<commit_message>
[Shubham] Update code in Jan
</commit_message>
<xml_diff>
--- a/data/excel/FlightBooking.xlsx
+++ b/data/excel/FlightBooking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\projectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C440B55-620D-4596-A72B-8986F11260A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A010C44-C265-448E-B855-DD2E7F37822A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet14" sheetId="72" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Sheet7" sheetId="81" r:id="rId7"/>
     <sheet name="Sheet6" sheetId="80" r:id="rId8"/>
     <sheet name="Sheet5" sheetId="79" r:id="rId9"/>
+    <sheet name="Sheet8" sheetId="83" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4702" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4836" uniqueCount="403">
   <si>
     <t>del</t>
   </si>
@@ -1247,6 +1248,12 @@
   </si>
   <si>
     <t>8-Mar-2024</t>
+  </si>
+  <si>
+    <t>24B,9E,6E,12E</t>
+  </si>
+  <si>
+    <t>29-Jan-2024</t>
   </si>
 </sst>
 </file>
@@ -5992,6 +5999,585 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E64D9A7-538F-4A91-A281-E05404AC9E04}">
+  <dimension ref="A1:BV2"/>
+  <sheetViews>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AS2" sqref="AS2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB1" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC1" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="AD1" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE1" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="AF1" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN1" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="AO1" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AU1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV1" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AW1" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="AX1" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="AY1" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="AZ1" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="BA1" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="BB1" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="BC1" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="BD1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="BE1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="BF1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="BG1" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="BH1" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="BI1" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="BJ1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="BK1" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="BL1" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="BM1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="BN1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="BO1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="BP1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="BQ1" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="BR1" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="BS1" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="BT1" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="BU1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="BV1" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:74" ht="48" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="1">
+        <v>3</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB2" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC2" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AD2" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="AE2" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO2" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT2" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AV2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AY2" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="AZ2" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BA2" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="BB2" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="BC2" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BD2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BE2" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BF2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BG2" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BJ2" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BK2" s="7">
+        <v>123</v>
+      </c>
+      <c r="BL2" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BM2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BN2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BO2" s="9">
+        <v>1</v>
+      </c>
+      <c r="BP2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BQ2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BR2" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BS2" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BT2" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BU2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BV2" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2" xr:uid="{0CD54666-EFDC-4C33-BF78-76EF6476D710}">
+      <formula1>"bom,maa,dxb"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{44ACB44D-92E3-46C1-B853-FB349BC606BA}">
+      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{0D536917-8DDC-4DC9-8190-D64021CE5DC7}">
+      <formula1>"sbt,preprod117,Live"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AT2" xr:uid="{F348DDAF-17B0-45BF-8A89-91C706F36CA4}">
+      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2" xr:uid="{A98ADDC0-87E0-4C28-804B-0EE4B741AA5A}">
+      <formula1>"1,2,3,4,5,6"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BG2" xr:uid="{4899AA23-9D78-4609-8B4D-7E95C61E2192}">
+      <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{14FFAEE5-838A-40C6-A868-3EEF0E4F7A5F}">
+      <formula1>"Laxmi@123,Password@123,Quad@720,Quad@721"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{748048FB-E074-4A81-AF08-D0E22C4A4999}">
+      <formula1>"Saurav_at,tarun"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{42DBF49A-ABDB-4433-A6C0-3F7DDEF1FDC4}">
+      <formula1>"at,QL"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{FF3333FC-9C0C-4E2E-A451-FF174DAC3490}">
+      <formula1>"//staging117/backoffice/,//preprod.quadlabs.net/backoffice/,//test.quadlabs.net/backoffice/"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2" xr:uid="{ACEBCA11-95B3-474B-9D84-CF84766EE043}">
+      <formula1>"Old,New"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2" xr:uid="{81F3A335-5865-4402-9854-20EA212FDB9A}">
+      <formula1>"prince.chaurasia@quadlabs.com,Gunjan.swain@quadlabs.com,laxmi.khanal@quadlabs.com,shubham.natkar@quadlabs.com,piyush.chauhan@quadlabs.com,ankur.yadav@quadlabs.com,sachin.kumar@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2" xr:uid="{A12E1609-25BB-4994-97A0-25D9D3B36AEC}">
+      <formula1>"InPolicy,OutPolicy,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2 AG2" xr:uid="{4E0A9ED7-EAC9-4CAC-8AAF-107BABE2C722}">
+      <formula1>"1,2,3,4,5,6,7,8"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX2" xr:uid="{60E61AA3-AC62-4092-9CEF-AEC79C51FCC3}">
+      <formula1>"Flight,Flight+Hotel,Flight+Car,Flight+Hotel+Car,Flight+Car+Hotel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2" xr:uid="{9206C22A-AD82-499A-8D35-EC7904C28788}">
+      <formula1>"OneWay,RoundTrip"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{E80A7C73-0EC1-4A31-B681-3D8CEEA65FBF}">
+      <formula1>"Domestic,International"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2" xr:uid="{30E9077C-0BAE-484C-8800-EF1CF1F7AC72}">
+      <formula1>"Individual,Guest,Personal,Dependent"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ2" xr:uid="{F0728136-07B8-4DCB-8931-8286C1B5114F}">
+      <formula1>"Master Card,Visa"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2" xr:uid="{79D15FF4-E890-48B2-95E9-B925300F5696}">
+      <formula1>"0,1,2,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2:AK2" xr:uid="{7A4026AA-3BD3-4AEB-9FB4-D4314AADBC3A}">
+      <formula1>"0,1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{B56167FE-47C9-4A65-9086-DF87F9515F4E}">
+      <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2 AF2 BN2" xr:uid="{25D1A8B3-725F-4BE3-9BEA-65FEA3721120}">
+      <formula1>"Applied,NotApplied"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BV2" xr:uid="{87D7DF79-5693-494C-872E-DB134D2656A4}">
+      <formula1>"Shubham Natkar,Laxmi Khanal,Sudesh Kumar"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{9C6B7A26-5793-477F-88FC-541C38102924}">
+      <formula1>"sbt,preprod117"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{FD073124-14C7-453E-9EBE-2942304264F9}">
+      <formula1>"Administrator,Travel Arranger,Employee"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BL2" xr:uid="{6B11E2D2-8B91-497D-BDCC-CC90F8522260}">
+      <formula1>"Trip Request,Flight Book,Addtocart"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BQ2" xr:uid="{647EAA93-2B4A-46AD-9D99-968D39FC469E}">
+      <formula1>"Hold and quote,Quote,Fullfillment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2 AP2" xr:uid="{055CAE79-5247-4886-ADFA-BB6E2D01E952}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2" xr:uid="{F6717E76-07CE-4958-9239-247A1BBF1E1B}">
+      <formula1>"On,Off"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AR2" xr:uid="{8EC77805-5CBE-4970-810E-3F3A7B8C691D}">
+      <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2" xr:uid="{344D26CF-4F2A-4587-9D46-1E751217A884}">
+      <formula1>"Business trip  - Without reason"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{F238780C-3877-4C40-9ADD-1BAF2F3F0FBE}">
+      <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{2E3A18E1-980E-4149-8CB1-EFF96A8811C3}">
+      <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{240CC697-928A-4105-8DA3-8BB81E5D6CD9}">
+      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="shubham.natkar@quadlabs.com" xr:uid="{FAD7C1B9-42CA-4064-B9E8-01C6858CDC14}"/>
+    <hyperlink ref="G2" r:id="rId2" display="Password@123" xr:uid="{E4072722-AAB4-4707-AFCC-638E300E309A}"/>
+    <hyperlink ref="U2" r:id="rId3" display="prince.chaurasia@quadlabs.com" xr:uid="{1D6A9996-E1EA-4781-92FB-8CE3C9232EFF}"/>
+    <hyperlink ref="Q2" r:id="rId4" display="Admin@123" xr:uid="{623772FD-EAD4-45C8-9F6D-B43DF26977DD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98DCEC8-5D14-41F2-ACA0-1145C7751169}">
   <dimension ref="A1:BN5"/>
@@ -16152,8 +16738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873E93BB-9FC7-4764-85A0-340252AC8F16}">
   <dimension ref="A1:BV13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AF8" sqref="AF8"/>
+    <sheetView topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="BA2" sqref="BA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16670,7 +17256,7 @@
         <v>153</v>
       </c>
       <c r="BS2" s="7" t="s">
-        <v>304</v>
+        <v>401</v>
       </c>
       <c r="BT2" s="7" t="s">
         <v>145</v>
@@ -19957,8 +20543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4687B7CB-B79C-4A10-A96F-CB8129CC90D6}">
   <dimension ref="A1:BV5"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20316,7 +20902,7 @@
         <v>295</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>59</v>
+        <v>156</v>
       </c>
       <c r="S2" s="8" t="s">
         <v>192</v>
@@ -20352,7 +20938,7 @@
         <v>246</v>
       </c>
       <c r="AD2" s="12" t="s">
-        <v>350</v>
+        <v>385</v>
       </c>
       <c r="AE2" s="12" t="s">
         <v>306</v>
@@ -20540,7 +21126,7 @@
         <v>295</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>59</v>
+        <v>156</v>
       </c>
       <c r="S3" s="8" t="s">
         <v>192</v>
@@ -20576,7 +21162,7 @@
         <v>246</v>
       </c>
       <c r="AD3" s="12" t="s">
-        <v>308</v>
+        <v>402</v>
       </c>
       <c r="AE3" s="12" t="s">
         <v>306</v>
@@ -20764,7 +21350,7 @@
         <v>295</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>59</v>
+        <v>156</v>
       </c>
       <c r="S4" s="8" t="s">
         <v>192</v>
@@ -20988,7 +21574,7 @@
         <v>295</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>59</v>
+        <v>156</v>
       </c>
       <c r="S5" s="8" t="s">
         <v>192</v>
@@ -21024,7 +21610,7 @@
         <v>246</v>
       </c>
       <c r="AD5" s="12" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="AE5" s="12" t="s">
         <v>386</v>

</xml_diff>

<commit_message>
[Shubham] Update SSO login
</commit_message>
<xml_diff>
--- a/data/excel/FlightBooking.xlsx
+++ b/data/excel/FlightBooking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\projectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A010C44-C265-448E-B855-DD2E7F37822A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C8AA87-190E-490F-8133-74621778D432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet14" sheetId="72" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4836" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4842" uniqueCount="409">
   <si>
     <t>del</t>
   </si>
@@ -1254,6 +1254,24 @@
   </si>
   <si>
     <t>29-Jan-2024</t>
+  </si>
+  <si>
+    <t>//test.quadlabs.net/SSO_Login</t>
+  </si>
+  <si>
+    <t>LoginType</t>
+  </si>
+  <si>
+    <t>SSO</t>
+  </si>
+  <si>
+    <t>Emailid</t>
+  </si>
+  <si>
+    <t>SDN</t>
+  </si>
+  <si>
+    <t>test.quadlabs.net</t>
   </si>
 </sst>
 </file>
@@ -1383,7 +1401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1466,6 +1484,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6001,18 +6022,94 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E64D9A7-538F-4A91-A281-E05404AC9E04}">
-  <dimension ref="A1:BV2"/>
+  <dimension ref="A1:BY2"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AS2" sqref="AS2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="39" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="14" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="9" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>35</v>
       </c>
@@ -6050,193 +6147,202 @@
         <v>15</v>
       </c>
       <c r="M1" s="29" t="s">
+        <v>404</v>
+      </c>
+      <c r="N1" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="O1" s="29" t="s">
+        <v>406</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="Q1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="R1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="S1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="T1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="U1" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="S1" s="23" t="s">
+      <c r="V1" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="T1" s="23" t="s">
+      <c r="W1" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="U1" s="23" t="s">
+      <c r="X1" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="23" t="s">
+      <c r="Y1" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="W1" s="23" t="s">
+      <c r="Z1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="23" t="s">
+      <c r="AA1" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="Y1" s="23" t="s">
+      <c r="AB1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="23" t="s">
+      <c r="AC1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="23" t="s">
+      <c r="AD1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="AB1" s="23" t="s">
+      <c r="AE1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="23" t="s">
+      <c r="AF1" s="23" t="s">
         <v>245</v>
       </c>
-      <c r="AD1" s="24" t="s">
+      <c r="AG1" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AE1" s="24" t="s">
+      <c r="AH1" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AI1" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="AG1" s="19" t="s">
+      <c r="AJ1" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AH1" s="19" t="s">
+      <c r="AK1" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AI1" s="23" t="s">
+      <c r="AL1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="AJ1" s="23" t="s">
+      <c r="AM1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="AK1" s="23" t="s">
+      <c r="AN1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="AL1" s="23" t="s">
+      <c r="AO1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="AM1" s="23" t="s">
+      <c r="AP1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="AN1" s="23" t="s">
+      <c r="AQ1" s="23" t="s">
         <v>287</v>
       </c>
-      <c r="AO1" s="23" t="s">
+      <c r="AR1" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="AU1" s="23" t="s">
+      <c r="AX1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="AV1" s="23" t="s">
+      <c r="AY1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="AW1" s="23" t="s">
+      <c r="AZ1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="AX1" s="23" t="s">
+      <c r="BA1" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="AY1" s="33" t="s">
+      <c r="BB1" s="33" t="s">
         <v>310</v>
       </c>
-      <c r="AZ1" s="33" t="s">
+      <c r="BC1" s="33" t="s">
         <v>311</v>
       </c>
-      <c r="BA1" s="33" t="s">
+      <c r="BD1" s="33" t="s">
         <v>312</v>
       </c>
-      <c r="BB1" s="33" t="s">
+      <c r="BE1" s="33" t="s">
         <v>313</v>
       </c>
-      <c r="BC1" s="23" t="s">
+      <c r="BF1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="BD1" s="23" t="s">
+      <c r="BG1" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="BE1" s="23" t="s">
+      <c r="BH1" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="BF1" s="23" t="s">
+      <c r="BI1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="BG1" s="23" t="s">
+      <c r="BJ1" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="BH1" s="14" t="s">
+      <c r="BK1" s="14" t="s">
         <v>323</v>
       </c>
-      <c r="BI1" s="14" t="s">
+      <c r="BL1" s="14" t="s">
         <v>324</v>
       </c>
-      <c r="BJ1" s="23" t="s">
+      <c r="BM1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="BK1" s="23" t="s">
+      <c r="BN1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="BL1" s="23" t="s">
+      <c r="BO1" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="BM1" s="23" t="s">
+      <c r="BP1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="BN1" s="19" t="s">
+      <c r="BQ1" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="BO1" s="19" t="s">
+      <c r="BR1" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="BP1" s="19" t="s">
+      <c r="BS1" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="BQ1" s="23" t="s">
+      <c r="BT1" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="BR1" s="23" t="s">
+      <c r="BU1" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="BS1" s="23" t="s">
+      <c r="BV1" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="BT1" s="23" t="s">
+      <c r="BW1" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="BU1" s="23" t="s">
+      <c r="BX1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="BV1" s="23" t="s">
+      <c r="BY1" s="23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:74" ht="48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:77" ht="48" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
@@ -6274,210 +6380,219 @@
         <v>45</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>296</v>
+        <v>405</v>
       </c>
       <c r="N2" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="O2" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="Q2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="U2" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="V2" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="W2" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="X2" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="Y2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="Z2" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="AA2" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="Y2" s="7" t="s">
+      <c r="AB2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="AC2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="AD2" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="AB2" s="28" t="s">
+      <c r="AE2" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="AC2" s="30" t="s">
+      <c r="AF2" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="AD2" s="12" t="s">
+      <c r="AG2" s="12" t="s">
         <v>385</v>
       </c>
-      <c r="AE2" s="12" t="s">
+      <c r="AH2" s="12" t="s">
         <v>306</v>
       </c>
-      <c r="AF2" s="9" t="s">
+      <c r="AI2" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="AG2" s="1">
+      <c r="AJ2" s="1">
         <v>3</v>
       </c>
-      <c r="AH2" s="10" t="s">
+      <c r="AK2" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="AI2" s="1">
+      <c r="AL2" s="1">
         <v>2</v>
       </c>
-      <c r="AJ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="7" t="s">
+      <c r="AM2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AN2" s="7" t="s">
+      <c r="AQ2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AO2" s="7">
+      <c r="AR2" s="7">
         <v>0</v>
       </c>
-      <c r="AP2" s="13" t="s">
+      <c r="AS2" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="AQ2" s="7" t="s">
+      <c r="AT2" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="AR2" s="7" t="s">
+      <c r="AU2" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="AS2" s="13" t="s">
+      <c r="AV2" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="AT2" s="13" t="s">
+      <c r="AW2" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="AU2" s="7">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="7">
-        <v>1</v>
-      </c>
-      <c r="AW2" s="7">
-        <v>1</v>
-      </c>
-      <c r="AX2" s="7" t="s">
+      <c r="AX2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AZ2" s="7">
+        <v>1</v>
+      </c>
+      <c r="BA2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AY2" s="13" t="s">
+      <c r="BB2" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="AZ2" s="13" t="s">
+      <c r="BC2" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="BA2" s="34" t="s">
+      <c r="BD2" s="34" t="s">
         <v>314</v>
       </c>
-      <c r="BB2" s="34" t="s">
+      <c r="BE2" s="34" t="s">
         <v>315</v>
       </c>
-      <c r="BC2" s="7">
+      <c r="BF2" s="7">
         <v>78554432323</v>
       </c>
-      <c r="BD2" s="7" t="s">
+      <c r="BG2" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="BE2" s="7">
+      <c r="BH2" s="7">
         <v>345678</v>
       </c>
-      <c r="BF2" s="7" t="s">
+      <c r="BI2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="BG2" s="7" t="s">
+      <c r="BJ2" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="BH2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI2" s="1" t="s">
+      <c r="BK2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BL2" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="BJ2" s="7" t="s">
+      <c r="BM2" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="BK2" s="7">
+      <c r="BN2" s="7">
         <v>123</v>
       </c>
-      <c r="BL2" s="7" t="s">
+      <c r="BO2" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="BM2" s="7" t="s">
+      <c r="BP2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="BN2" s="9" t="s">
+      <c r="BQ2" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="BO2" s="9">
-        <v>1</v>
-      </c>
-      <c r="BP2" s="9" t="s">
+      <c r="BR2" s="9">
+        <v>1</v>
+      </c>
+      <c r="BS2" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="BQ2" s="7" t="s">
+      <c r="BT2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="BR2" s="32" t="s">
+      <c r="BU2" s="32" t="s">
         <v>281</v>
       </c>
-      <c r="BS2" s="7" t="s">
+      <c r="BV2" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="BT2" s="7" t="s">
+      <c r="BW2" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="BU2" s="7" t="s">
+      <c r="BX2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="BV2" s="11" t="s">
+      <c r="BY2" s="11" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="35">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2" xr:uid="{0CD54666-EFDC-4C33-BF78-76EF6476D710}">
+  <dataValidations count="36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2" xr:uid="{0CD54666-EFDC-4C33-BF78-76EF6476D710}">
       <formula1>"bom,maa,dxb"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{44ACB44D-92E3-46C1-B853-FB349BC606BA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2" xr:uid="{44ACB44D-92E3-46C1-B853-FB349BC606BA}">
       <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{0D536917-8DDC-4DC9-8190-D64021CE5DC7}">
       <formula1>"sbt,preprod117,Live"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AT2" xr:uid="{F348DDAF-17B0-45BF-8A89-91C706F36CA4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV2:AW2" xr:uid="{F348DDAF-17B0-45BF-8A89-91C706F36CA4}">
       <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2" xr:uid="{A98ADDC0-87E0-4C28-804B-0EE4B741AA5A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2" xr:uid="{A98ADDC0-87E0-4C28-804B-0EE4B741AA5A}">
       <formula1>"1,2,3,4,5,6"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BG2" xr:uid="{4899AA23-9D78-4609-8B4D-7E95C61E2192}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ2" xr:uid="{4899AA23-9D78-4609-8B4D-7E95C61E2192}">
       <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{14FFAEE5-838A-40C6-A868-3EEF0E4F7A5F}">
@@ -6492,87 +6607,91 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{FF3333FC-9C0C-4E2E-A451-FF174DAC3490}">
       <formula1>"//staging117/backoffice/,//preprod.quadlabs.net/backoffice/,//test.quadlabs.net/backoffice/"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2" xr:uid="{ACEBCA11-95B3-474B-9D84-CF84766EE043}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{ACEBCA11-95B3-474B-9D84-CF84766EE043}">
       <formula1>"Old,New"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2" xr:uid="{81F3A335-5865-4402-9854-20EA212FDB9A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2" xr:uid="{81F3A335-5865-4402-9854-20EA212FDB9A}">
       <formula1>"prince.chaurasia@quadlabs.com,Gunjan.swain@quadlabs.com,laxmi.khanal@quadlabs.com,shubham.natkar@quadlabs.com,piyush.chauhan@quadlabs.com,ankur.yadav@quadlabs.com,sachin.kumar@quadlabs.com"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2" xr:uid="{A12E1609-25BB-4994-97A0-25D9D3B36AEC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2" xr:uid="{A12E1609-25BB-4994-97A0-25D9D3B36AEC}">
       <formula1>"InPolicy,OutPolicy,Null"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2 AG2" xr:uid="{4E0A9ED7-EAC9-4CAC-8AAF-107BABE2C722}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2 AJ2" xr:uid="{4E0A9ED7-EAC9-4CAC-8AAF-107BABE2C722}">
       <formula1>"1,2,3,4,5,6,7,8"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX2" xr:uid="{60E61AA3-AC62-4092-9CEF-AEC79C51FCC3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BA2" xr:uid="{60E61AA3-AC62-4092-9CEF-AEC79C51FCC3}">
       <formula1>"Flight,Flight+Hotel,Flight+Car,Flight+Hotel+Car,Flight+Car+Hotel"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2" xr:uid="{9206C22A-AD82-499A-8D35-EC7904C28788}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2" xr:uid="{9206C22A-AD82-499A-8D35-EC7904C28788}">
       <formula1>"OneWay,RoundTrip"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{E80A7C73-0EC1-4A31-B681-3D8CEEA65FBF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2" xr:uid="{E80A7C73-0EC1-4A31-B681-3D8CEEA65FBF}">
       <formula1>"Domestic,International"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2" xr:uid="{30E9077C-0BAE-484C-8800-EF1CF1F7AC72}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2" xr:uid="{30E9077C-0BAE-484C-8800-EF1CF1F7AC72}">
       <formula1>"Individual,Guest,Personal,Dependent"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ2" xr:uid="{F0728136-07B8-4DCB-8931-8286C1B5114F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BM2" xr:uid="{F0728136-07B8-4DCB-8931-8286C1B5114F}">
       <formula1>"Master Card,Visa"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2" xr:uid="{79D15FF4-E890-48B2-95E9-B925300F5696}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{79D15FF4-E890-48B2-95E9-B925300F5696}">
       <formula1>"0,1,2,Null"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2:AK2" xr:uid="{7A4026AA-3BD3-4AEB-9FB4-D4314AADBC3A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AN2" xr:uid="{7A4026AA-3BD3-4AEB-9FB4-D4314AADBC3A}">
       <formula1>"0,1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{B56167FE-47C9-4A65-9086-DF87F9515F4E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2" xr:uid="{B56167FE-47C9-4A65-9086-DF87F9515F4E}">
       <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2 AF2 BN2" xr:uid="{25D1A8B3-725F-4BE3-9BEA-65FEA3721120}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2 AI2 BQ2" xr:uid="{25D1A8B3-725F-4BE3-9BEA-65FEA3721120}">
       <formula1>"Applied,NotApplied"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BV2" xr:uid="{87D7DF79-5693-494C-872E-DB134D2656A4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BY2" xr:uid="{87D7DF79-5693-494C-872E-DB134D2656A4}">
       <formula1>"Shubham Natkar,Laxmi Khanal,Sudesh Kumar"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{9C6B7A26-5793-477F-88FC-541C38102924}">
       <formula1>"sbt,preprod117"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{FD073124-14C7-453E-9EBE-2942304264F9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{FD073124-14C7-453E-9EBE-2942304264F9}">
       <formula1>"Administrator,Travel Arranger,Employee"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BL2" xr:uid="{6B11E2D2-8B91-497D-BDCC-CC90F8522260}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BO2" xr:uid="{6B11E2D2-8B91-497D-BDCC-CC90F8522260}">
       <formula1>"Trip Request,Flight Book,Addtocart"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BQ2" xr:uid="{647EAA93-2B4A-46AD-9D99-968D39FC469E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BT2" xr:uid="{647EAA93-2B4A-46AD-9D99-968D39FC469E}">
       <formula1>"Hold and quote,Quote,Fullfillment"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2 AP2" xr:uid="{055CAE79-5247-4886-ADFA-BB6E2D01E952}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BU2 AS2" xr:uid="{055CAE79-5247-4886-ADFA-BB6E2D01E952}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2" xr:uid="{F6717E76-07CE-4958-9239-247A1BBF1E1B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2" xr:uid="{F6717E76-07CE-4958-9239-247A1BBF1E1B}">
       <formula1>"On,Off"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AR2" xr:uid="{8EC77805-5CBE-4970-810E-3F3A7B8C691D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AT2:AU2" xr:uid="{8EC77805-5CBE-4970-810E-3F3A7B8C691D}">
       <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2" xr:uid="{344D26CF-4F2A-4587-9D46-1E751217A884}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2" xr:uid="{344D26CF-4F2A-4587-9D46-1E751217A884}">
       <formula1>"Business trip  - Without reason"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{F238780C-3877-4C40-9ADD-1BAF2F3F0FBE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{F238780C-3877-4C40-9ADD-1BAF2F3F0FBE}">
       <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{2E3A18E1-980E-4149-8CB1-EFF96A8811C3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2" xr:uid="{2E3A18E1-980E-4149-8CB1-EFF96A8811C3}">
       <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{240CC697-928A-4105-8DA3-8BB81E5D6CD9}">
-      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{240CC697-928A-4105-8DA3-8BB81E5D6CD9}">
+      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{906F570E-507D-420C-940E-278E4EFCB370}">
+      <formula1>"Normal,SSO"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="shubham.natkar@quadlabs.com" xr:uid="{FAD7C1B9-42CA-4064-B9E8-01C6858CDC14}"/>
     <hyperlink ref="G2" r:id="rId2" display="Password@123" xr:uid="{E4072722-AAB4-4707-AFCC-638E300E309A}"/>
-    <hyperlink ref="U2" r:id="rId3" display="prince.chaurasia@quadlabs.com" xr:uid="{1D6A9996-E1EA-4781-92FB-8CE3C9232EFF}"/>
-    <hyperlink ref="Q2" r:id="rId4" display="Admin@123" xr:uid="{623772FD-EAD4-45C8-9F6D-B43DF26977DD}"/>
+    <hyperlink ref="X2" r:id="rId3" xr:uid="{1D6A9996-E1EA-4781-92FB-8CE3C9232EFF}"/>
+    <hyperlink ref="T2" r:id="rId4" display="Admin@123" xr:uid="{623772FD-EAD4-45C8-9F6D-B43DF26977DD}"/>
+    <hyperlink ref="O2" r:id="rId5" xr:uid="{41AF3579-0A29-47FF-A6EE-C017BADA9515}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20543,8 +20662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4687B7CB-B79C-4A10-A96F-CB8129CC90D6}">
   <dimension ref="A1:BV5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[Shubham] Update code on 09/1/24
</commit_message>
<xml_diff>
--- a/data/excel/FlightBooking.xlsx
+++ b/data/excel/FlightBooking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\projectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6F3F13-304B-401C-9405-F01AAAA00D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB758B67-C4AC-4132-A371-958A2095AC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet14" sheetId="72" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Sheet6" sheetId="80" r:id="rId8"/>
     <sheet name="Sheet5" sheetId="79" r:id="rId9"/>
     <sheet name="Sheet8" sheetId="83" r:id="rId10"/>
+    <sheet name="Sheet9" sheetId="84" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4844" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4986" uniqueCount="418">
   <si>
     <t>del</t>
   </si>
@@ -1275,6 +1276,30 @@
   </si>
   <si>
     <t>UpgradePolicy</t>
+  </si>
+  <si>
+    <t>Istanbul,Turkey - Ataturk (IST)</t>
+  </si>
+  <si>
+    <t>IST</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
+    <t>20-Feb-2024</t>
+  </si>
+  <si>
+    <t>John F Kennedy-United States,United States - John F. Kennedy International Airport (JFK)</t>
+  </si>
+  <si>
+    <t>JFK</t>
+  </si>
+  <si>
+    <t>23-Mar-2024</t>
+  </si>
+  <si>
+    <t>ankit.bist@quadlabs.com</t>
   </si>
 </sst>
 </file>
@@ -1774,7 +1799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B98EDDB2-6BE4-45F6-80CF-17F0C90DBF6A}">
   <dimension ref="A1:IT5"/>
   <sheetViews>
-    <sheetView topLeftCell="IF1" workbookViewId="0">
+    <sheetView topLeftCell="GW1" workbookViewId="0">
       <selection activeCell="IX10" sqref="IX10"/>
     </sheetView>
   </sheetViews>
@@ -6027,8 +6052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E64D9A7-538F-4A91-A281-E05404AC9E04}">
   <dimension ref="A1:BZ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AG8" sqref="AG8"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6426,28 +6451,28 @@
         <v>32</v>
       </c>
       <c r="Z2" s="7" t="s">
-        <v>132</v>
+        <v>412</v>
       </c>
       <c r="AA2" s="7" t="s">
         <v>337</v>
       </c>
       <c r="AB2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="7" t="s">
-        <v>33</v>
+        <v>140</v>
+      </c>
+      <c r="AC2" s="28" t="s">
+        <v>141</v>
       </c>
       <c r="AD2" s="7" t="s">
-        <v>140</v>
+        <v>411</v>
       </c>
       <c r="AE2" s="28" t="s">
-        <v>141</v>
+        <v>410</v>
       </c>
       <c r="AF2" s="30" t="s">
         <v>246</v>
       </c>
       <c r="AG2" s="12" t="s">
-        <v>385</v>
+        <v>413</v>
       </c>
       <c r="AH2" s="12" t="s">
         <v>306</v>
@@ -6586,7 +6611,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="36">
+  <dataValidations count="37">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2" xr:uid="{44ACB44D-92E3-46C1-B853-FB349BC606BA}">
       <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
     </dataValidation>
@@ -6693,6 +6718,9 @@
       <formula1>"Normal,SSO"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2" xr:uid="{9FCC3812-0A78-4C4A-83E4-5D06690FD278}">
+      <formula1>"bom,maa,dxb,IST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2" xr:uid="{0963ED60-77A7-4A2B-972F-564D84EB353B}">
       <formula1>"bom,maa,dxb"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6707,12 +6735,695 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B8F8D0-D766-4C64-AE8A-3BA802829F0D}">
+  <dimension ref="A1:BZ2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T28" sqref="T28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="91.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="9" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>404</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="29" t="s">
+        <v>406</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA1" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE1" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF1" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="AG1" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH1" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="AI1" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AN1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ1" s="23" t="s">
+        <v>409</v>
+      </c>
+      <c r="AR1" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="AS1" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AY1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ1" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="BA1" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="BB1" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="BC1" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="BD1" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="BE1" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="BF1" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="BG1" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="BH1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="BI1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="BJ1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="BK1" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="BL1" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="BM1" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="BN1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="BO1" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="BP1" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="BQ1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="BR1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="BS1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="BT1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="BU1" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="BV1" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="BW1" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="BX1" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="BY1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="BZ1" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:78" ht="48" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="1">
+        <v>3</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="O2" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="X2" s="35" t="s">
+        <v>417</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="AE2" s="28" t="s">
+        <v>414</v>
+      </c>
+      <c r="AF2" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AG2" s="12" t="s">
+        <v>416</v>
+      </c>
+      <c r="AH2" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ2" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AR2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS2" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AU2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AV2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AW2" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AX2" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AY2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AZ2" s="7">
+        <v>1</v>
+      </c>
+      <c r="BA2" s="7">
+        <v>1</v>
+      </c>
+      <c r="BB2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="BC2" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BD2" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BE2" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="BF2" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="BG2" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BH2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BI2" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BJ2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BK2" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BL2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN2" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BO2" s="7">
+        <v>123</v>
+      </c>
+      <c r="BP2" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BQ2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BR2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS2" s="9">
+        <v>1</v>
+      </c>
+      <c r="BT2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BU2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BV2" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BW2" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BX2" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BY2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BZ2" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2" xr:uid="{90D93D37-9C22-4698-841C-FED041DB87F4}">
+      <formula1>"bom,maa,dxb,IST,JFK"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{CC8FB706-3951-4250-A1E3-3F76870C3D4A}">
+      <formula1>"Normal,SSO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{5F72F893-A0D9-49CE-9690-EA3857459A4B}">
+      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2" xr:uid="{4BB6D6BE-D014-42D0-8A34-C47166523A09}">
+      <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{859917FD-E0A7-4F2C-BD1F-68DA2DAE983E}">
+      <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2" xr:uid="{D219607C-F2C5-4A38-8201-D27FCCCF93DB}">
+      <formula1>"Business trip  - Without reason"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2:AV2" xr:uid="{A12CD16C-6418-4FCF-BEF4-4418845D1213}">
+      <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2" xr:uid="{C3905F57-1B7E-4EFA-94DA-7233652F7F8E}">
+      <formula1>"On,Off"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BV2 AT2 AQ2" xr:uid="{45F185F8-31EC-46B1-ABEA-7635A86AF516}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BU2" xr:uid="{4211F050-602B-4387-B682-25E54593032C}">
+      <formula1>"Hold and quote,Quote,Fullfillment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BP2" xr:uid="{4A09CD01-C341-4F4F-80BB-444A72B05334}">
+      <formula1>"Trip Request,Flight Book,Addtocart"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{191D4A16-78A5-44DA-BA3F-58BF1723743E}">
+      <formula1>"Administrator,Travel Arranger,Employee"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{5232188D-F0A8-4076-A51D-966AEDFB2183}">
+      <formula1>"sbt,preprod117"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BZ2" xr:uid="{ADC4A5DE-F1FA-4A98-8EB7-A982B9AAF89E}">
+      <formula1>"Shubham Natkar,Laxmi Khanal,Sudesh Kumar"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2 AI2 BR2" xr:uid="{5FDACED2-9ABD-43D2-9CED-79F874056968}">
+      <formula1>"Applied,NotApplied"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2" xr:uid="{D9D47D60-260D-438A-AB1A-E7640E8E4A5E}">
+      <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AN2" xr:uid="{DC2884CA-7498-46CA-9CFC-A006097F85D9}">
+      <formula1>"0,1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{1B782B1A-99FD-4AF0-BDAB-3075214F0073}">
+      <formula1>"0,1,2,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BN2" xr:uid="{E6A79FF1-EAD5-4279-B608-B03A7417761F}">
+      <formula1>"Master Card,Visa"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2" xr:uid="{0BFE0387-361E-427C-8B6C-3FF618079EE1}">
+      <formula1>"Individual,Guest,Personal,Dependent"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2" xr:uid="{29043126-83A7-4918-BB54-BF5A2F6FC08C}">
+      <formula1>"Domestic,International"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2" xr:uid="{07E2FA78-B5AD-4996-AD8B-E488D53EBDDF}">
+      <formula1>"OneWay,RoundTrip"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB2" xr:uid="{B864253E-50C3-4EBF-B35F-3CA34D0B4043}">
+      <formula1>"Flight,Flight+Hotel,Flight+Car,Flight+Hotel+Car,Flight+Car+Hotel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2 AJ2" xr:uid="{0ACB26FA-66BE-4A93-A38A-80A0846BCAB1}">
+      <formula1>"1,2,3,4,5,6,7,8"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{59316F6A-741F-42FE-8C9A-3C183ADEB28B}">
+      <formula1>"InPolicy,OutPolicy,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2" xr:uid="{634DF8F1-B130-4428-95AC-9CC9E18FA097}">
+      <formula1>"prince.chaurasia@quadlabs.com,Gunjan.swain@quadlabs.com,laxmi.khanal@quadlabs.com,shubham.natkar@quadlabs.com,piyush.chauhan@quadlabs.com,ankur.yadav@quadlabs.com,sachin.kumar@quadlabs.com,ankit.bist@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{60855C35-0E78-4BB1-9975-BAA2C1FC5735}">
+      <formula1>"Old,New"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{DA60ACC0-5F1C-42CE-BBAE-8D9176E2B731}">
+      <formula1>"//staging117/backoffice/,//preprod.quadlabs.net/backoffice/,//test.quadlabs.net/backoffice/"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{85D7396F-6DC0-4CA6-800E-6C803F2CC1C5}">
+      <formula1>"at,QL"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{6761D887-2E90-44EA-979F-5ADE262186ED}">
+      <formula1>"Saurav_at,tarun"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{DBA551E6-DBEE-421C-A4E1-9E979D097BDE}">
+      <formula1>"Laxmi@123,Password@123,Quad@720,Quad@721"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2" xr:uid="{BBD5C23F-817F-487F-B51E-F17B617C805F}">
+      <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BL2" xr:uid="{2324EC73-740B-4CF1-8709-97F369E3BA25}">
+      <formula1>"1,2,3,4,5,6"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW2:AX2" xr:uid="{8B8AEAF0-A3F4-4129-AF02-8FB49E1FA39B}">
+      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{5FB86278-861C-4B78-8178-3F76A1AD926D}">
+      <formula1>"sbt,preprod117,Live"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2" xr:uid="{E895117B-1E23-469C-BCD3-A206E37C7DF6}">
+      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="shubham.natkar@quadlabs.com" xr:uid="{507B0C3A-98E8-43ED-B1EF-2899D7BF9618}"/>
+    <hyperlink ref="G2" r:id="rId2" display="Password@123" xr:uid="{886A0FA7-BB3F-46E7-A9B9-3B8C1CD6877E}"/>
+    <hyperlink ref="X2" r:id="rId3" display="shubham.natkar@quadlabs.com" xr:uid="{5F68D4CD-1312-434D-AE49-F1844CE02EB2}"/>
+    <hyperlink ref="T2" r:id="rId4" display="Admin@123" xr:uid="{2378CC3D-FD6B-43B1-A253-5A5B5BB517F8}"/>
+    <hyperlink ref="O2" r:id="rId5" xr:uid="{3535D123-5873-4A23-9A27-C7AD9EA638D9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98DCEC8-5D14-41F2-ACA0-1145C7751169}">
   <dimension ref="A1:BN5"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AC6" sqref="AC6"/>
+      <selection activeCell="V2" sqref="V2:W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20673,7 +21384,7 @@
   <dimension ref="A1:BV5"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4:AB4"/>
+      <selection activeCell="Y5" sqref="Y5:Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[Shubham] Code on More product with Add to cart
</commit_message>
<xml_diff>
--- a/data/excel/FlightBooking.xlsx
+++ b/data/excel/FlightBooking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankur.Yadav\git\ProjectQuadlabs\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham.Natkar\git\ProjectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6C0EF9-62B9-4D4B-8A5D-6EFE8514AD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C758AA-2912-42E9-BC97-20C293E4F627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="12600" yWindow="4335" windowWidth="16200" windowHeight="11415" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="14" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet14" sheetId="72" r:id="rId1"/>
@@ -30,8 +30,9 @@
     <sheet name="TestLCC+Gds" sheetId="90" r:id="rId15"/>
     <sheet name="Filtersheet" sheetId="91" r:id="rId16"/>
     <sheet name="Branding" sheetId="92" r:id="rId17"/>
-    <sheet name="NonBranding" sheetId="96" r:id="rId18"/>
-    <sheet name="Sheet17" sheetId="95" r:id="rId19"/>
+    <sheet name="Sheet11" sheetId="97" r:id="rId18"/>
+    <sheet name="NonBranding" sheetId="96" r:id="rId19"/>
+    <sheet name="Sheet17" sheetId="95" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8307" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8443" uniqueCount="520">
   <si>
     <t>del</t>
   </si>
@@ -16865,8 +16866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8274BB29-8D16-41B7-801E-EA95E6FC3C79}">
   <dimension ref="A1:BW8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2:AB2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18884,6 +18885,654 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1152101-88D1-47D8-974F-BB578AD00182}">
+  <dimension ref="A1:BW2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="BJ19" sqref="BJ19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="36" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="14" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>404</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>406</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA1" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB1" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC1" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK1" s="23" t="s">
+        <v>409</v>
+      </c>
+      <c r="AL1" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="AM1" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN1" s="23" t="s">
+        <v>478</v>
+      </c>
+      <c r="AO1" s="23" t="s">
+        <v>477</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="AV1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW1" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AX1" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="AY1" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="AZ1" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="BA1" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="BB1" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="BC1" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="BD1" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="BE1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="BF1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="BG1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="BH1" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="BI1" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="BJ1" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="BK1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="BL1" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="BM1" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="BN1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="BO1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="BS1" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="BT1" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="BU1" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="BV1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="BW1" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I2" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="R2" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z2" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA2" s="12" t="s">
+        <v>506</v>
+      </c>
+      <c r="AB2" s="12" t="s">
+        <v>511</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK2" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM2" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO2" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP2" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT2" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU2" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ2" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA2" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB2" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC2" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD2" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF2" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH2" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK2" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL2" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM2" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BN2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP2" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS2" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="BT2" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU2" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW2" s="7" t="s">
+        <v>432</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{25F60164-562A-48E3-8AC1-3D4314AA16B5}">
+      <formula1>"prince.chaurasia@quadlabs.com,ayushi.shivhare@quadlabs.com,laxmi.khanal@quadlabs.com,shubham.natkar@quadlabs.com,piyush.chauhan@quadlabs.com,ankur.yadav@quadlabs.com,sachin.kumar@quadlabs.com,ankit.bist@quadlabs.com,ajit.kumar@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2" xr:uid="{FB2E7975-C45A-4044-A09D-01478BE0CC22}">
+      <formula1>"LCC,LCC+GDS,GDS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{D4A070FA-90F0-401D-86ED-16885515AA57}">
+      <formula1>"Normal,SSO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{6C219D70-C84D-470D-91F5-D75280927F82}">
+      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{505A1FAB-445B-4B08-983E-70B20B60B500}">
+      <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2 BW2" xr:uid="{249F9713-76F2-4AC8-A20A-C618293667D2}">
+      <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur,D Divaker S,Ankur Yadav,Sachin Kumar"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2" xr:uid="{C79C0E2B-0A1B-4D2A-8611-22A143F5AEF4}">
+      <formula1>"Business trip  - Without reason"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AR2" xr:uid="{5E9A6754-E241-46E2-B2D3-ED802818109F}">
+      <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{FADB8C77-ED57-4B66-9920-593FC152E36D}">
+      <formula1>"On,Off"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP2 AK2 AN2 BS2" xr:uid="{5E566F18-E6EF-40D8-91E5-BDA76AB29C03}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2" xr:uid="{76FE0F58-E3FC-451E-9372-CF10DBD4D5A3}">
+      <formula1>"Hold and quote,Quote,Fullfillment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BM2" xr:uid="{CFEEC431-62CF-4087-A2D1-A5F9EDC2291E}">
+      <formula1>"Trip Request,Flight Book,Addtocart"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{060E6A03-C224-4062-A54C-F69844C41AC3}">
+      <formula1>"Administrator,Travel Arranger,Employee"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{86BE20C5-805B-4B6A-9B03-9C1026FF1459}">
+      <formula1>"sbt,preprod117"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2 BO2 C2" xr:uid="{BC362102-86DA-491E-92AB-BB7399F63F17}">
+      <formula1>"Applied,NotApplied"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{E1DB1DAA-3729-49E6-A990-CAD6084A96CC}">
+      <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AH2" xr:uid="{EB980B71-C557-4420-9F4E-8A2694C1CDA9}">
+      <formula1>"0,1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{972F423D-F1D5-40DE-BC56-9CA1436471F0}">
+      <formula1>"0,1,2,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2" xr:uid="{DF49684E-C672-4142-BCEB-84EA90241E0B}">
+      <formula1>"Master Card,Visa"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2" xr:uid="{6F3686EE-246B-4DB4-BB11-02C3EC33819F}">
+      <formula1>"Individual,Guest,Personal,Dependent"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2" xr:uid="{DAD87662-E6E8-40DD-92C4-979C8552F30A}">
+      <formula1>"Domestic,International"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2" xr:uid="{7702B831-421E-4B60-9C57-C800F7B8A6D9}">
+      <formula1>"OneWay,RoundTrip"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2" xr:uid="{3A64760F-D34B-4E60-AE36-BE71C7676729}">
+      <formula1>"Flight,Flight+Hotel,Flight+Car,Flight+Hotel+Car,Flight+Car+Hotel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2 D2" xr:uid="{617A75F5-B873-470F-8224-2F5FA6AA66C3}">
+      <formula1>"1,2,3,4,5,6,7,8"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2" xr:uid="{546C0649-2FA6-49D3-AD11-F2EAD1C45578}">
+      <formula1>"InPolicy,OutPolicy,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{2AE44249-D30A-45F0-98EC-A8512DED6FDB}">
+      <formula1>"Old,New"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2" xr:uid="{FE062D84-BF61-47F5-BCBF-634752FF4142}">
+      <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2" xr:uid="{D35036CE-2CFC-431F-9845-AEEF9CDC8F61}">
+      <formula1>"1,2,3,4,5,6"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{FD4E3DD2-6FE5-4556-ACB9-7C3B3648902A}">
+      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AT2" xr:uid="{BEE93905-D711-45DD-81F0-C3D752C20B57}">
+      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare,ECO LITE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2" xr:uid="{AA58A214-4C3E-4476-8784-656901C29FE0}">
+      <formula1>"Duration,Layover,TimingFilter"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{E0BA27C0-A15A-42BC-92AB-33294D8BE26D}">
+      <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com,ankit.singh@quadlabs.com"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" display="Admin@123" xr:uid="{ECEDCFC7-0E34-4131-B791-2108DA5D8FDE}"/>
+    <hyperlink ref="I2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{59BA13CB-A0B3-4C25-9305-4D382065537B}"/>
+    <hyperlink ref="R2" r:id="rId3" display="ajit.kumar@quadlabs.com" xr:uid="{C2C28B64-9E94-4C43-AEAA-6BF3B5C9590E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B5143E-7EC1-42F1-ACFE-7B1A3D040ECA}">
   <dimension ref="A1:BW7"/>
   <sheetViews>
@@ -20674,7 +21323,1187 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98DCEC8-5D14-41F2-ACA0-1145C7751169}">
+  <dimension ref="A1:BN5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="39" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:66" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="Y1" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA1" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI1" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="AJ1" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AP1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ1" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR1" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="AS1" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="AT1" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="AU1" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="AV1" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="AW1" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="AX1" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="AY1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AZ1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="BA1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="BB1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="BC1" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="BD1" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="BE1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="BF1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="BG1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="BI1" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="BJ1" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="BK1" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="BL1" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="BM1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="BN1" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:66" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="W2" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="X2" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="Z2" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ2" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AL2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AM2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AN2" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AO2" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AP2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="AT2" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="AU2" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="AV2" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="AW2" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="AX2" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="AY2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AZ2" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BA2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB2" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BC2" s="7">
+        <v>123</v>
+      </c>
+      <c r="BD2" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BE2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BF2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BG2" s="9">
+        <v>1</v>
+      </c>
+      <c r="BH2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BJ2" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BK2" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BL2" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BM2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN2" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:66" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="W3" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="X3" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="Y3" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="Z3" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="AA3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ3" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AL3" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AM3" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AN3" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AO3" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AP3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS3" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="AT3" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="AU3" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="AV3" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="AW3" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="AX3" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="AY3" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AZ3" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BA3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB3" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BC3" s="7">
+        <v>123</v>
+      </c>
+      <c r="BD3" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BE3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BF3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BG3" s="9">
+        <v>1</v>
+      </c>
+      <c r="BH3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BJ3" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BK3" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BL3" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BM3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN3" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:66" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="W4" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="X4" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="Y4" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="Z4" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="AA4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC4" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ4" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AL4" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AM4" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AN4" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AO4" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AP4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS4" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="AT4" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="AU4" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="AV4" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="AW4" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="AX4" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="AY4" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AZ4" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BA4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB4" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BC4" s="7">
+        <v>123</v>
+      </c>
+      <c r="BD4" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BE4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BF4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BG4" s="9">
+        <v>1</v>
+      </c>
+      <c r="BH4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BJ4" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BK4" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BL4" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BM4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN4" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:66" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="W5" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="X5" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="Y5" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="Z5" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="AA5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC5" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ5" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AL5" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AM5" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AN5" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AO5" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AP5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS5" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="AT5" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="AU5" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="AV5" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="AW5" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="AX5" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="AY5" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AZ5" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BA5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB5" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BC5" s="7">
+        <v>123</v>
+      </c>
+      <c r="BD5" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BE5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BF5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BG5" s="9">
+        <v>1</v>
+      </c>
+      <c r="BH5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BJ5" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BK5" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BL5" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BM5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN5" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2:AO5" xr:uid="{4C45BBA0-2468-4129-8909-5E2815C4EB44}">
+      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O5" xr:uid="{0498C7EF-6BD5-4414-BC0D-0B89B42C81D9}">
+      <formula1>"Old,New"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P5" xr:uid="{6B5A5108-C256-4019-BCCE-CC490AE4BCA9}">
+      <formula1>"prince.chaurasia@quadlabs.com,Gunjan.swain@quadlabs.com,laxmi.khanal@quadlabs.com,shubham.natkar@quadlabs.com,piyush.chauhan@quadlabs.com,ankur.yadav@quadlabs.com,sachin.kumar@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2:AI5" xr:uid="{98E61256-8850-4C03-9D36-075015ED01CC}">
+      <formula1>"InPolicy,OutPolicy,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB5 E2:E5" xr:uid="{9059B3F4-968D-45C1-9427-4E4FCE205F4A}">
+      <formula1>"1,2,3,4,5,6,7,8"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AS5" xr:uid="{077F7F65-7BB5-4FF2-8522-DB49E74D3F7B}">
+      <formula1>"Flight,Flight+Hotel,Flight+Car,Flight+Hotel+Car,Flight+Car+Hotel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S5" xr:uid="{E25BF804-2BBA-4031-9ABA-3A22A0457AF3}">
+      <formula1>"OneWay,RoundTrip"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R5" xr:uid="{1C07EC02-53F8-470A-B793-1B536FCB9483}">
+      <formula1>"Domestic,International"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q5" xr:uid="{45B43896-196B-444E-A57D-D4CF1B7E05FC}">
+      <formula1>"Individual,Guest,Personal,Dependent"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB2:BB5" xr:uid="{35A02EEF-3CF7-4406-BF54-46DCB8DA4267}">
+      <formula1>"Master Card,Visa"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ2:AJ5" xr:uid="{355C1A6D-9AEA-4E38-A8A2-D07607C65B9F}">
+      <formula1>"0,1,2,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AF5" xr:uid="{FF4C6D12-8499-48C6-9435-8BF7F2942144}">
+      <formula1>"0,1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M5" xr:uid="{464D4F95-3883-47A0-A7F9-51D1446597F9}">
+      <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF2:BF5 AA2:AA5 D2:D5" xr:uid="{CC07C336-4A16-45DF-9638-834263C42DA1}">
+      <formula1>"Applied,NotApplied"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BN2:BN5" xr:uid="{4BE857CC-3145-4D79-8C91-EDE9B44EFC75}">
+      <formula1>"Shubham Natkar,Laxmi Khanal,Sudesh Kumar"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5 C2:C5" xr:uid="{3BCDF557-BCA7-4EC3-BCE9-519CC0BE82C9}">
+      <formula1>"sbt,preprod117"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J5" xr:uid="{BE80B1B3-5276-4F1B-BB3A-635D81D89A1D}">
+      <formula1>"Administrator,Travel Arranger,Employee"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BD2:BD5" xr:uid="{95D2C220-28DD-4E70-871A-BFF40ED3F615}">
+      <formula1>"Trip Request,Flight Book,Addtocart"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2:BI5" xr:uid="{46FC40F7-467A-4BD0-98E6-97E1DFD7992D}">
+      <formula1>"Hold and quote,Quote,Fullfillment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK2:AK5 BJ2:BJ5" xr:uid="{2F077DC4-B127-4A6C-B83E-A983439A5C56}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N5" xr:uid="{87705A5D-5904-48F2-97F2-09BBE7E4C9E5}">
+      <formula1>"On,Off"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AM5" xr:uid="{21E7CB9D-A18E-45EE-A9A7-7913A0D2CA86}">
+      <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X5" xr:uid="{C72D7F70-CA7A-4ABD-AC3C-9E2D040E2C72}">
+      <formula1>"Business trip  - Without reason"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I5" xr:uid="{310C9F88-970E-4677-8A0C-823F3944E930}">
+      <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K5" xr:uid="{1F86D526-37BB-4AB6-9484-49FD291F83B4}">
+      <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L5" xr:uid="{529624DA-8D2C-417A-901F-39F2D5A560C2}">
+      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H5" xr:uid="{472D9684-51F0-4B7F-BCE6-F0A4853100BE}">
+      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V5" xr:uid="{D31D6128-9BD3-4BF2-B783-90C7D458BF1B}">
+      <formula1>"bom,maa,dxb"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="P2" r:id="rId1" display="prince.chaurasia@quadlabs.com" xr:uid="{A9E84B22-2915-495B-AECF-AAC5DAE73BB0}"/>
+    <hyperlink ref="L2" r:id="rId2" display="Admin@123" xr:uid="{F51E4D43-C8EB-438B-B592-AADCA801EF4A}"/>
+    <hyperlink ref="P3" r:id="rId3" display="prince.chaurasia@quadlabs.com" xr:uid="{A42925E6-506D-491F-A2F9-F455B650502B}"/>
+    <hyperlink ref="L3" r:id="rId4" display="Admin@123" xr:uid="{42E2827C-4AE1-40E8-9D44-6A4766CA39B8}"/>
+    <hyperlink ref="P4" r:id="rId5" display="prince.chaurasia@quadlabs.com" xr:uid="{4AF26D49-4895-4F3E-9ED2-9D46678B1705}"/>
+    <hyperlink ref="L4" r:id="rId6" display="Admin@123" xr:uid="{1941C053-7D7B-4DE5-8719-5729011254F8}"/>
+    <hyperlink ref="P5" r:id="rId7" display="prince.chaurasia@quadlabs.com" xr:uid="{618D8B16-3569-4302-B345-E33A90DAF425}"/>
+    <hyperlink ref="L5" r:id="rId8" display="Admin@123" xr:uid="{64B90536-6371-4F46-948E-8188EA7B4DE9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E4DC434-9680-44B9-B67E-2B0017A95C76}">
   <dimension ref="A1:BW2"/>
   <sheetViews>
@@ -21317,1186 +23146,6 @@
     <hyperlink ref="N2" r:id="rId1" display="Admin@123" xr:uid="{7F0E7733-1EF9-43C3-8A77-5B1C27FAD025}"/>
     <hyperlink ref="I2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{BB2DB6D9-9D3D-40A8-8CB4-F2B30B699183}"/>
     <hyperlink ref="R2" r:id="rId3" display="ajit.kumar@quadlabs.com" xr:uid="{55D73720-9660-4207-9DE0-6DF75728F9D4}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98DCEC8-5D14-41F2-ACA0-1145C7751169}">
-  <dimension ref="A1:BN5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="39" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="15.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:66" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="O1" s="23" t="s">
-        <v>291</v>
-      </c>
-      <c r="P1" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="R1" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="S1" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="T1" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="W1" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="X1" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="Y1" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z1" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="AA1" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB1" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC1" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD1" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="AE1" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF1" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG1" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="AH1" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI1" s="23" t="s">
-        <v>287</v>
-      </c>
-      <c r="AJ1" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="AP1" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="AQ1" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="AR1" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="AS1" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="AT1" s="33" t="s">
-        <v>310</v>
-      </c>
-      <c r="AU1" s="33" t="s">
-        <v>311</v>
-      </c>
-      <c r="AV1" s="33" t="s">
-        <v>312</v>
-      </c>
-      <c r="AW1" s="33" t="s">
-        <v>313</v>
-      </c>
-      <c r="AX1" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="AY1" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="AZ1" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="BA1" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="BB1" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="BC1" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="BD1" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="BE1" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="BF1" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="BG1" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH1" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="BI1" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="BJ1" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="BK1" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="BL1" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="BM1" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="BN1" s="23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:66" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="1">
-        <v>3</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="V2" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="W2" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="X2" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>294</v>
-      </c>
-      <c r="Z2" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>3</v>
-      </c>
-      <c r="AC2" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="AD2" s="1">
-        <v>2</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ2" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="AL2" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="AM2" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="AN2" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="AO2" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="AP2" s="7">
-        <v>1</v>
-      </c>
-      <c r="AQ2" s="7">
-        <v>1</v>
-      </c>
-      <c r="AR2" s="7">
-        <v>1</v>
-      </c>
-      <c r="AS2" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="AT2" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="AU2" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="AV2" s="34" t="s">
-        <v>314</v>
-      </c>
-      <c r="AW2" s="34" t="s">
-        <v>315</v>
-      </c>
-      <c r="AX2" s="7">
-        <v>78554432323</v>
-      </c>
-      <c r="AY2" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="AZ2" s="7">
-        <v>345678</v>
-      </c>
-      <c r="BA2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="BB2" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="BC2" s="7">
-        <v>123</v>
-      </c>
-      <c r="BD2" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="BE2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="BF2" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="BG2" s="9">
-        <v>1</v>
-      </c>
-      <c r="BH2" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="BI2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="BJ2" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="BK2" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="BL2" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="BM2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="BN2" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:66" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="1">
-        <v>3</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="V3" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="W3" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="X3" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="Y3" s="12" t="s">
-        <v>294</v>
-      </c>
-      <c r="Z3" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="AA3" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>3</v>
-      </c>
-      <c r="AC3" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="AD3" s="1">
-        <v>2</v>
-      </c>
-      <c r="AE3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI3" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="AL3" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="AM3" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="AN3" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="AO3" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="AP3" s="7">
-        <v>1</v>
-      </c>
-      <c r="AQ3" s="7">
-        <v>1</v>
-      </c>
-      <c r="AR3" s="7">
-        <v>1</v>
-      </c>
-      <c r="AS3" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="AT3" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="AU3" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="AV3" s="34" t="s">
-        <v>314</v>
-      </c>
-      <c r="AW3" s="34" t="s">
-        <v>315</v>
-      </c>
-      <c r="AX3" s="7">
-        <v>78554432323</v>
-      </c>
-      <c r="AY3" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="AZ3" s="7">
-        <v>345678</v>
-      </c>
-      <c r="BA3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="BB3" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="BC3" s="7">
-        <v>123</v>
-      </c>
-      <c r="BD3" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="BE3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="BF3" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="BG3" s="9">
-        <v>1</v>
-      </c>
-      <c r="BH3" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="BI3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="BJ3" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="BK3" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="BL3" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="BM3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="BN3" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:66" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="W4" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="X4" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="Y4" s="12" t="s">
-        <v>294</v>
-      </c>
-      <c r="Z4" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="AA4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB4" s="1">
-        <v>3</v>
-      </c>
-      <c r="AC4" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="AD4" s="1">
-        <v>2</v>
-      </c>
-      <c r="AE4" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF4" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI4" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ4" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="AL4" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="AM4" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="AN4" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="AO4" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="AP4" s="7">
-        <v>1</v>
-      </c>
-      <c r="AQ4" s="7">
-        <v>1</v>
-      </c>
-      <c r="AR4" s="7">
-        <v>1</v>
-      </c>
-      <c r="AS4" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="AT4" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="AU4" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="AV4" s="34" t="s">
-        <v>314</v>
-      </c>
-      <c r="AW4" s="34" t="s">
-        <v>315</v>
-      </c>
-      <c r="AX4" s="7">
-        <v>78554432323</v>
-      </c>
-      <c r="AY4" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="AZ4" s="7">
-        <v>345678</v>
-      </c>
-      <c r="BA4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="BB4" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="BC4" s="7">
-        <v>123</v>
-      </c>
-      <c r="BD4" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="BE4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="BF4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="BG4" s="9">
-        <v>1</v>
-      </c>
-      <c r="BH4" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="BI4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="BJ4" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="BK4" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="BL4" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="BM4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="BN4" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:66" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="1">
-        <v>3</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="S5" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="T5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="V5" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="W5" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="X5" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="Y5" s="12" t="s">
-        <v>294</v>
-      </c>
-      <c r="Z5" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="AA5" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB5" s="1">
-        <v>3</v>
-      </c>
-      <c r="AC5" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="AD5" s="1">
-        <v>2</v>
-      </c>
-      <c r="AE5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI5" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="AL5" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="AM5" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="AN5" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="AO5" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="AP5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AQ5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AR5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AS5" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="AT5" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="AU5" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="AV5" s="34" t="s">
-        <v>314</v>
-      </c>
-      <c r="AW5" s="34" t="s">
-        <v>315</v>
-      </c>
-      <c r="AX5" s="7">
-        <v>78554432323</v>
-      </c>
-      <c r="AY5" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="AZ5" s="7">
-        <v>345678</v>
-      </c>
-      <c r="BA5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="BB5" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="BC5" s="7">
-        <v>123</v>
-      </c>
-      <c r="BD5" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="BE5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="BF5" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="BG5" s="9">
-        <v>1</v>
-      </c>
-      <c r="BH5" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="BI5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="BJ5" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="BK5" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="BL5" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="BM5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="BN5" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="28">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2:AO5" xr:uid="{4C45BBA0-2468-4129-8909-5E2815C4EB44}">
-      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O5" xr:uid="{0498C7EF-6BD5-4414-BC0D-0B89B42C81D9}">
-      <formula1>"Old,New"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P5" xr:uid="{6B5A5108-C256-4019-BCCE-CC490AE4BCA9}">
-      <formula1>"prince.chaurasia@quadlabs.com,Gunjan.swain@quadlabs.com,laxmi.khanal@quadlabs.com,shubham.natkar@quadlabs.com,piyush.chauhan@quadlabs.com,ankur.yadav@quadlabs.com,sachin.kumar@quadlabs.com"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2:AI5" xr:uid="{98E61256-8850-4C03-9D36-075015ED01CC}">
-      <formula1>"InPolicy,OutPolicy,Null"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB5 E2:E5" xr:uid="{9059B3F4-968D-45C1-9427-4E4FCE205F4A}">
-      <formula1>"1,2,3,4,5,6,7,8"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AS5" xr:uid="{077F7F65-7BB5-4FF2-8522-DB49E74D3F7B}">
-      <formula1>"Flight,Flight+Hotel,Flight+Car,Flight+Hotel+Car,Flight+Car+Hotel"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S5" xr:uid="{E25BF804-2BBA-4031-9ABA-3A22A0457AF3}">
-      <formula1>"OneWay,RoundTrip"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R5" xr:uid="{1C07EC02-53F8-470A-B793-1B536FCB9483}">
-      <formula1>"Domestic,International"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q5" xr:uid="{45B43896-196B-444E-A57D-D4CF1B7E05FC}">
-      <formula1>"Individual,Guest,Personal,Dependent"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB2:BB5" xr:uid="{35A02EEF-3CF7-4406-BF54-46DCB8DA4267}">
-      <formula1>"Master Card,Visa"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ2:AJ5" xr:uid="{355C1A6D-9AEA-4E38-A8A2-D07607C65B9F}">
-      <formula1>"0,1,2,Null"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AF5" xr:uid="{FF4C6D12-8499-48C6-9435-8BF7F2942144}">
-      <formula1>"0,1,2,3,4,5"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M5" xr:uid="{464D4F95-3883-47A0-A7F9-51D1446597F9}">
-      <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF2:BF5 AA2:AA5 D2:D5" xr:uid="{CC07C336-4A16-45DF-9638-834263C42DA1}">
-      <formula1>"Applied,NotApplied"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BN2:BN5" xr:uid="{4BE857CC-3145-4D79-8C91-EDE9B44EFC75}">
-      <formula1>"Shubham Natkar,Laxmi Khanal,Sudesh Kumar"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5 C2:C5" xr:uid="{3BCDF557-BCA7-4EC3-BCE9-519CC0BE82C9}">
-      <formula1>"sbt,preprod117"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J5" xr:uid="{BE80B1B3-5276-4F1B-BB3A-635D81D89A1D}">
-      <formula1>"Administrator,Travel Arranger,Employee"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BD2:BD5" xr:uid="{95D2C220-28DD-4E70-871A-BFF40ED3F615}">
-      <formula1>"Trip Request,Flight Book,Addtocart"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2:BI5" xr:uid="{46FC40F7-467A-4BD0-98E6-97E1DFD7992D}">
-      <formula1>"Hold and quote,Quote,Fullfillment"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK2:AK5 BJ2:BJ5" xr:uid="{2F077DC4-B127-4A6C-B83E-A983439A5C56}">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N5" xr:uid="{87705A5D-5904-48F2-97F2-09BBE7E4C9E5}">
-      <formula1>"On,Off"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AM5" xr:uid="{21E7CB9D-A18E-45EE-A9A7-7913A0D2CA86}">
-      <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X5" xr:uid="{C72D7F70-CA7A-4ABD-AC3C-9E2D040E2C72}">
-      <formula1>"Business trip  - Without reason"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I5" xr:uid="{310C9F88-970E-4677-8A0C-823F3944E930}">
-      <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K5" xr:uid="{1F86D526-37BB-4AB6-9484-49FD291F83B4}">
-      <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L5" xr:uid="{529624DA-8D2C-417A-901F-39F2D5A560C2}">
-      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H5" xr:uid="{472D9684-51F0-4B7F-BCE6-F0A4853100BE}">
-      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V5" xr:uid="{D31D6128-9BD3-4BF2-B783-90C7D458BF1B}">
-      <formula1>"bom,maa,dxb"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" display="prince.chaurasia@quadlabs.com" xr:uid="{A9E84B22-2915-495B-AECF-AAC5DAE73BB0}"/>
-    <hyperlink ref="L2" r:id="rId2" display="Admin@123" xr:uid="{F51E4D43-C8EB-438B-B592-AADCA801EF4A}"/>
-    <hyperlink ref="P3" r:id="rId3" display="prince.chaurasia@quadlabs.com" xr:uid="{A42925E6-506D-491F-A2F9-F455B650502B}"/>
-    <hyperlink ref="L3" r:id="rId4" display="Admin@123" xr:uid="{42E2827C-4AE1-40E8-9D44-6A4766CA39B8}"/>
-    <hyperlink ref="P4" r:id="rId5" display="prince.chaurasia@quadlabs.com" xr:uid="{4AF26D49-4895-4F3E-9ED2-9D46678B1705}"/>
-    <hyperlink ref="L4" r:id="rId6" display="Admin@123" xr:uid="{1941C053-7D7B-4DE5-8719-5729011254F8}"/>
-    <hyperlink ref="P5" r:id="rId7" display="prince.chaurasia@quadlabs.com" xr:uid="{618D8B16-3569-4302-B345-E33A90DAF425}"/>
-    <hyperlink ref="L5" r:id="rId8" display="Admin@123" xr:uid="{64B90536-6371-4F46-948E-8188EA7B4DE9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[Ankur] Code on Add to cart for non branding
</commit_message>
<xml_diff>
--- a/data/excel/FlightBooking.xlsx
+++ b/data/excel/FlightBooking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham.Natkar\git\ProjectQuadlabs\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankur.Yadav\git\ProjectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C758AA-2912-42E9-BC97-20C293E4F627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED004B1-1A6E-4510-8A92-1AAFF7C7BBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="14" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="14" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet14" sheetId="72" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8443" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8443" uniqueCount="523">
   <si>
     <t>del</t>
   </si>
@@ -1615,6 +1615,15 @@
   </si>
   <si>
     <t>piyush.chauhan@quadlabs.com</t>
+  </si>
+  <si>
+    <t>28-Nov-2024</t>
+  </si>
+  <si>
+    <t>26-Nov-2024</t>
+  </si>
+  <si>
+    <t>Master Card</t>
   </si>
 </sst>
 </file>
@@ -18888,8 +18897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1152101-88D1-47D8-974F-BB578AD00182}">
   <dimension ref="A1:BW2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="BJ19" sqref="BJ19"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22507,8 +22516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E4DC434-9680-44B9-B67E-2B0017A95C76}">
   <dimension ref="A1:BW2"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
+      <selection activeCell="BP15" sqref="BP15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22539,7 +22548,7 @@
     <col min="25" max="25" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="25.85546875" bestFit="1" customWidth="1"/>
@@ -22574,7 +22583,7 @@
     <col min="60" max="60" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="9" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -22878,7 +22887,7 @@
         <v>132</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>137</v>
+        <v>337</v>
       </c>
       <c r="V2" s="7" t="s">
         <v>484</v>
@@ -22896,10 +22905,10 @@
         <v>246</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="AB2" s="12" t="s">
-        <v>508</v>
+        <v>520</v>
       </c>
       <c r="AC2" s="9" t="s">
         <v>69</v>
@@ -22956,7 +22965,7 @@
         <v>292</v>
       </c>
       <c r="AU2" s="13" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="AV2" s="7">
         <v>1</v>
@@ -23004,13 +23013,13 @@
         <v>156</v>
       </c>
       <c r="BK2" s="7" t="s">
-        <v>290</v>
+        <v>522</v>
       </c>
       <c r="BL2" s="7">
         <v>123</v>
       </c>
       <c r="BM2" s="7" t="s">
-        <v>451</v>
+        <v>150</v>
       </c>
       <c r="BN2" s="7" t="s">
         <v>34</v>
@@ -23044,6 +23053,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="32">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2" xr:uid="{D3900C6F-1777-4D0B-830B-6CA38C678C2E}">
       <formula1>"LCC,LCC+GDS,GDS"</formula1>

</xml_diff>

<commit_message>
"New code for staging 117 [Ankur yadav]
</commit_message>
<xml_diff>
--- a/data/excel/FlightBooking.xlsx
+++ b/data/excel/FlightBooking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankur.Yadav\git\ProjectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED004B1-1A6E-4510-8A92-1AAFF7C7BBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E823AB96-25D8-410C-9C7E-6B1017DCDD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="14" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="12" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet14" sheetId="72" r:id="rId1"/>
@@ -30,9 +30,10 @@
     <sheet name="TestLCC+Gds" sheetId="90" r:id="rId15"/>
     <sheet name="Filtersheet" sheetId="91" r:id="rId16"/>
     <sheet name="Branding" sheetId="92" r:id="rId17"/>
-    <sheet name="Sheet11" sheetId="97" r:id="rId18"/>
+    <sheet name="Branding118" sheetId="97" r:id="rId18"/>
     <sheet name="NonBranding" sheetId="96" r:id="rId19"/>
-    <sheet name="Sheet17" sheetId="95" r:id="rId20"/>
+    <sheet name="Nonbranding117" sheetId="95" r:id="rId20"/>
+    <sheet name="Test117" sheetId="99" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8443" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9016" uniqueCount="547">
   <si>
     <t>del</t>
   </si>
@@ -1617,13 +1618,85 @@
     <t>piyush.chauhan@quadlabs.com</t>
   </si>
   <si>
-    <t>28-Nov-2024</t>
-  </si>
-  <si>
-    <t>26-Nov-2024</t>
-  </si>
-  <si>
-    <t>Master Card</t>
+    <t>sachinkumar</t>
+  </si>
+  <si>
+    <t>Admin@123</t>
+  </si>
+  <si>
+    <t>ECO VALUE</t>
+  </si>
+  <si>
+    <t>ECONOMY COMFORT</t>
+  </si>
+  <si>
+    <t>4CJDOMEL9TNCR1R</t>
+  </si>
+  <si>
+    <t>27-Mar-2025</t>
+  </si>
+  <si>
+    <t>14-Apr-2025</t>
+  </si>
+  <si>
+    <t>27-Apr-2025</t>
+  </si>
+  <si>
+    <t>21-Apr-2025</t>
+  </si>
+  <si>
+    <t>23-Apr-2025</t>
+  </si>
+  <si>
+    <t>22-Apr-2025</t>
+  </si>
+  <si>
+    <t>25-Apr-2025</t>
+  </si>
+  <si>
+    <t>Verify Booking flow-International(One Way).</t>
+  </si>
+  <si>
+    <t>Verify Booking flow-International(Round Trip).</t>
+  </si>
+  <si>
+    <t>25-Mar-2025</t>
+  </si>
+  <si>
+    <t>26-Mar-2025</t>
+  </si>
+  <si>
+    <t>28-Mar-2025</t>
+  </si>
+  <si>
+    <t>6-Mar-2025</t>
+  </si>
+  <si>
+    <t>Oman Air</t>
+  </si>
+  <si>
+    <t>Chennai, Tamil Nadu, India (MAA-Chennai Intl.)</t>
+  </si>
+  <si>
+    <t>30-Mar-2025</t>
+  </si>
+  <si>
+    <t>Dubai,United Arab Emirates - Dubai  (DXB)</t>
+  </si>
+  <si>
+    <t>Verify Booking flow- (Flight+ Hotel)-International.</t>
+  </si>
+  <si>
+    <t>Verify Booking flow- (Flight+ Hotel)-Domestic.</t>
+  </si>
+  <si>
+    <t>Test on Flight+ Hotel 1</t>
+  </si>
+  <si>
+    <t>Test on Flight+ Hotel 2</t>
+  </si>
+  <si>
+    <t>16-Mar-2025</t>
   </si>
 </sst>
 </file>
@@ -16876,7 +16949,7 @@
   <dimension ref="A1:BW8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18895,16 +18968,16 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1152101-88D1-47D8-974F-BB578AD00182}">
-  <dimension ref="A1:BW2"/>
+  <dimension ref="A1:BW5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
@@ -18914,7 +18987,7 @@
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -18922,14 +18995,14 @@
     <col min="18" max="18" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="36" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="25.85546875" bestFit="1" customWidth="1"/>
@@ -19211,10 +19284,10 @@
         <v>36</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>500</v>
+        <v>452</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D2" s="1">
         <v>3</v>
@@ -19226,10 +19299,10 @@
         <v>3</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>403</v>
+        <v>296</v>
       </c>
       <c r="I2" s="35" t="s">
         <v>343</v>
@@ -19244,10 +19317,10 @@
         <v>52</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>44</v>
+        <v>520</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>295</v>
+        <v>521</v>
       </c>
       <c r="O2" s="8" t="s">
         <v>59</v>
@@ -19259,7 +19332,7 @@
         <v>293</v>
       </c>
       <c r="R2" s="35" t="s">
-        <v>343</v>
+        <v>519</v>
       </c>
       <c r="S2" s="7" t="s">
         <v>32</v>
@@ -19286,10 +19359,10 @@
         <v>246</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>506</v>
+        <v>534</v>
       </c>
       <c r="AB2" s="12" t="s">
-        <v>511</v>
+        <v>525</v>
       </c>
       <c r="AC2" s="9" t="s">
         <v>69</v>
@@ -19321,8 +19394,8 @@
       <c r="AL2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AM2" s="7">
-        <v>0</v>
+      <c r="AM2" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="AN2" s="13" t="s">
         <v>281</v>
@@ -19334,19 +19407,19 @@
         <v>153</v>
       </c>
       <c r="AQ2" s="7" t="s">
-        <v>139</v>
+        <v>414</v>
       </c>
       <c r="AR2" s="7" t="s">
-        <v>139</v>
+        <v>414</v>
       </c>
       <c r="AS2" s="13" t="s">
-        <v>292</v>
+        <v>522</v>
       </c>
       <c r="AT2" s="13" t="s">
-        <v>292</v>
+        <v>522</v>
       </c>
       <c r="AU2" s="13" t="s">
-        <v>498</v>
+        <v>129</v>
       </c>
       <c r="AV2" s="7">
         <v>1</v>
@@ -19418,7 +19491,7 @@
         <v>7</v>
       </c>
       <c r="BS2" s="32" t="s">
-        <v>153</v>
+        <v>281</v>
       </c>
       <c r="BT2" s="7" t="s">
         <v>304</v>
@@ -19433,109 +19506,796 @@
         <v>432</v>
       </c>
     </row>
+    <row r="3" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="R3" s="35" t="s">
+        <v>519</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="X3" s="36" t="s">
+        <v>449</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="Z3" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA3" s="12" t="s">
+        <v>526</v>
+      </c>
+      <c r="AB3" s="12" t="s">
+        <v>527</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK3" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN3" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO3" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP3" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ3" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="AR3" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="AS3" s="13" t="s">
+        <v>522</v>
+      </c>
+      <c r="AT3" s="13" t="s">
+        <v>522</v>
+      </c>
+      <c r="AU3" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AV3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ3" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA3" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB3" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC3" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD3" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE3" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF3" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH3" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK3" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL3" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM3" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BN3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP3" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS3" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT3" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU3" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW3" s="7" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="R4" s="35" t="s">
+        <v>519</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="Z4" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA4" s="12" t="s">
+        <v>528</v>
+      </c>
+      <c r="AB4" s="12" t="s">
+        <v>529</v>
+      </c>
+      <c r="AC4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK4" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN4" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO4" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ4" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="AR4" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="AS4" s="13" t="s">
+        <v>522</v>
+      </c>
+      <c r="AT4" s="13" t="s">
+        <v>522</v>
+      </c>
+      <c r="AU4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AV4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ4" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA4" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB4" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC4" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD4" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE4" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF4" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH4" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI4" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK4" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL4" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM4" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BN4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP4" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS4" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT4" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU4" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW4" s="7" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="5" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="R5" s="35" t="s">
+        <v>519</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="Z5" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA5" s="12" t="s">
+        <v>530</v>
+      </c>
+      <c r="AB5" s="12" t="s">
+        <v>531</v>
+      </c>
+      <c r="AC5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE5" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK5" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN5" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO5" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ5" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="AR5" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="AS5" s="13" t="s">
+        <v>522</v>
+      </c>
+      <c r="AT5" s="13" t="s">
+        <v>522</v>
+      </c>
+      <c r="AU5" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AV5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ5" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA5" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB5" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC5" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD5" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE5" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF5" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH5" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI5" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK5" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL5" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM5" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BN5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP5" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS5" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT5" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU5" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW5" s="7" t="s">
+        <v>432</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="32">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{25F60164-562A-48E3-8AC1-3D4314AA16B5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R5" xr:uid="{D1C29CB6-7D71-4C9F-AA7E-BCB27B558B9E}">
       <formula1>"prince.chaurasia@quadlabs.com,ayushi.shivhare@quadlabs.com,laxmi.khanal@quadlabs.com,shubham.natkar@quadlabs.com,piyush.chauhan@quadlabs.com,ankur.yadav@quadlabs.com,sachin.kumar@quadlabs.com,ankit.bist@quadlabs.com,ajit.kumar@quadlabs.com"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2" xr:uid="{FB2E7975-C45A-4044-A09D-01478BE0CC22}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2:AU5" xr:uid="{BCE20CB4-3431-457A-8EE0-9DFA5B7EC149}">
       <formula1>"LCC,LCC+GDS,GDS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{D4A070FA-90F0-401D-86ED-16885515AA57}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5" xr:uid="{99333616-1054-4CE3-803C-764BFFEDB27C}">
       <formula1>"Normal,SSO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{6C219D70-C84D-470D-91F5-D75280927F82}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H5" xr:uid="{F9353EFC-07AC-4B3B-98E8-69D81F4234B1}">
       <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{505A1FAB-445B-4B08-983E-70B20B60B500}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M5" xr:uid="{3F7C362B-2676-4E9F-A161-EE26C36383D0}">
       <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2 BW2" xr:uid="{249F9713-76F2-4AC8-A20A-C618293667D2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K5 BW2:BW5" xr:uid="{0CB11497-59A5-4089-A817-57E44F74594C}">
       <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur,D Divaker S,Ankur Yadav,Sachin Kumar"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2" xr:uid="{C79C0E2B-0A1B-4D2A-8611-22A143F5AEF4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z5" xr:uid="{BF8D8700-B723-433A-B31C-8816891F6AD1}">
       <formula1>"Business trip  - Without reason"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AR2" xr:uid="{5E9A6754-E241-46E2-B2D3-ED802818109F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AR5" xr:uid="{9D2B7538-80D7-431A-81A6-FE5C66B85211}">
       <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{FADB8C77-ED57-4B66-9920-593FC152E36D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P5" xr:uid="{07E1DC5A-5609-4805-9738-0A7B234AFF1C}">
       <formula1>"On,Off"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP2 AK2 AN2 BS2" xr:uid="{5E566F18-E6EF-40D8-91E5-BDA76AB29C03}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP2:AP5 AK2:AK5 AN2:AN5 BS2:BS5" xr:uid="{2CAC40F4-B0C8-4FAF-B3EF-FB8D74381C26}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2" xr:uid="{76FE0F58-E3FC-451E-9372-CF10DBD4D5A3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2:BR5" xr:uid="{BE696F33-88F6-4242-81D5-3A1231C471DC}">
       <formula1>"Hold and quote,Quote,Fullfillment"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BM2" xr:uid="{CFEEC431-62CF-4087-A2D1-A5F9EDC2291E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BM2:BM5" xr:uid="{6721F498-20BE-4E45-8A07-FFD6F3EDB5AC}">
       <formula1>"Trip Request,Flight Book,Addtocart"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{060E6A03-C224-4062-A54C-F69844C41AC3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L5" xr:uid="{431381AE-0088-4A2B-A9FB-62D5CE6B9B50}">
       <formula1>"Administrator,Travel Arranger,Employee"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{86BE20C5-805B-4B6A-9B03-9C1026FF1459}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5" xr:uid="{65E9D3A0-C2C4-4A5D-9F56-39913CD71534}">
       <formula1>"sbt,preprod117"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2 BO2 C2" xr:uid="{BC362102-86DA-491E-92AB-BB7399F63F17}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2:AC5 BO2:BO5 C2:C5" xr:uid="{8BEC20D9-6C20-4974-A3D2-1C9EAF6FCC47}">
       <formula1>"Applied,NotApplied"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{E1DB1DAA-3729-49E6-A990-CAD6084A96CC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O5" xr:uid="{DD0E79A3-9B04-4B10-B396-02C50DE24A48}">
       <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AH2" xr:uid="{EB980B71-C557-4420-9F4E-8A2694C1CDA9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AH5" xr:uid="{41E24847-3316-4D3B-B0D4-746E34A68E25}">
       <formula1>"0,1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{972F423D-F1D5-40DE-BC56-9CA1436471F0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2:AM5" xr:uid="{41A9908D-CFD5-4918-8067-4F85EC1B6759}">
       <formula1>"0,1,2,Null"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2" xr:uid="{DF49684E-C672-4142-BCEB-84EA90241E0B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2:BK5" xr:uid="{06385851-2E08-407E-8153-AC204078B183}">
       <formula1>"Master Card,Visa"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2" xr:uid="{6F3686EE-246B-4DB4-BB11-02C3EC33819F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S5" xr:uid="{E40B6617-1EEC-421D-A1E7-93FE69EF4B50}">
       <formula1>"Individual,Guest,Personal,Dependent"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2" xr:uid="{DAD87662-E6E8-40DD-92C4-979C8552F30A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T5" xr:uid="{448C40A0-04E0-4A20-B9CC-AA6D52EC4D83}">
       <formula1>"Domestic,International"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2" xr:uid="{7702B831-421E-4B60-9C57-C800F7B8A6D9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U5" xr:uid="{2774575B-E7EF-4180-854E-AE98655ACE51}">
       <formula1>"OneWay,RoundTrip"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2" xr:uid="{3A64760F-D34B-4E60-AE36-BE71C7676729}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2:AY5" xr:uid="{14C5715E-17CE-4034-A173-B5B9C696EA26}">
       <formula1>"Flight,Flight+Hotel,Flight+Car,Flight+Hotel+Car,Flight+Car+Hotel"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2 D2" xr:uid="{617A75F5-B873-470F-8224-2F5FA6AA66C3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD5 D2:D5" xr:uid="{2A8787A5-BF51-43C5-A1E5-8FF84DC787E2}">
       <formula1>"1,2,3,4,5,6,7,8"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2" xr:uid="{546C0649-2FA6-49D3-AD11-F2EAD1C45578}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL5" xr:uid="{3DEF7436-7DD1-469F-874C-E4A3CF3F0BFB}">
       <formula1>"InPolicy,OutPolicy,Null"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{2AE44249-D30A-45F0-98EC-A8512DED6FDB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q5" xr:uid="{4A7B71B2-7F0A-4FA2-8F79-4C9AF4029FCF}">
       <formula1>"Old,New"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2" xr:uid="{FE062D84-BF61-47F5-BCBF-634752FF4142}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2:BH5" xr:uid="{786455BA-80A4-40D3-B515-62977DA4529A}">
       <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2" xr:uid="{D35036CE-2CFC-431F-9845-AEEF9CDC8F61}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2:BI5" xr:uid="{4F3CD9F0-6EE0-45C0-BE68-A11D1FED42E9}">
       <formula1>"1,2,3,4,5,6"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{FD4E3DD2-6FE5-4556-ACB9-7C3B3648902A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2:AO5" xr:uid="{C5B07846-D033-4D7B-93DD-F602A6FECBF1}">
+      <formula1>"Duration,Layover,TimingFilter"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I5" xr:uid="{EC79C94A-F77B-4BEB-9FD2-2A007464EB43}">
+      <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com,ankit.singh@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N5" xr:uid="{AA68B074-32D7-4BC1-8328-71E7750EAEC3}">
       <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AT2" xr:uid="{BEE93905-D711-45DD-81F0-C3D752C20B57}">
-      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare,ECO LITE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2" xr:uid="{AA58A214-4C3E-4476-8784-656901C29FE0}">
-      <formula1>"Duration,Layover,TimingFilter"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{E0BA27C0-A15A-42BC-92AB-33294D8BE26D}">
-      <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com,ankit.singh@quadlabs.com"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AT5" xr:uid="{A64E5340-3DE2-44C0-A3F4-3939F0F8D110}">
+      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare,ECO LITE,ECO VALUE"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" display="Admin@123" xr:uid="{ECEDCFC7-0E34-4131-B791-2108DA5D8FDE}"/>
-    <hyperlink ref="I2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{59BA13CB-A0B3-4C25-9305-4D382065537B}"/>
-    <hyperlink ref="R2" r:id="rId3" display="ajit.kumar@quadlabs.com" xr:uid="{C2C28B64-9E94-4C43-AEAA-6BF3B5C9590E}"/>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{9D5E350B-B997-4B63-952B-E1D180F8B7F1}"/>
+    <hyperlink ref="I2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{79AB449E-9652-46F7-A3EE-4AFF97604D40}"/>
+    <hyperlink ref="R2" r:id="rId3" display="ajit.kumar@quadlabs.com" xr:uid="{26CA8F43-D419-4C2A-8CC6-230498F06E4D}"/>
+    <hyperlink ref="I3" r:id="rId4" display="shekhar.singh@quadlabs.com" xr:uid="{B3C6CE97-DF0A-473E-B433-6F32D321FBED}"/>
+    <hyperlink ref="R3" r:id="rId5" display="ajit.kumar@quadlabs.com" xr:uid="{C42F67E2-7AC6-444C-932F-9881BE76EACC}"/>
+    <hyperlink ref="I4:I5" r:id="rId6" display="shekhar.singh@quadlabs.com" xr:uid="{18A507A3-3F15-43DA-8D87-54261D8F7BE2}"/>
+    <hyperlink ref="R4:R5" r:id="rId7" display="ajit.kumar@quadlabs.com" xr:uid="{CF35DA78-8130-45B3-B773-B4AAD261A859}"/>
+    <hyperlink ref="N3:N5" r:id="rId8" display="Admin@123" xr:uid="{88351F86-4295-4738-87D0-D6A0373372F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19546,7 +20306,7 @@
   <dimension ref="A1:BW7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22514,10 +23274,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E4DC434-9680-44B9-B67E-2B0017A95C76}">
-  <dimension ref="A1:BW2"/>
+  <dimension ref="A1:BW5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
-      <selection activeCell="BP15" sqref="BP15"/>
+    <sheetView topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AL14" sqref="AL14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22534,7 +23294,7 @@
     <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -22598,7 +23358,7 @@
     <col min="75" max="75" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>35</v>
       </c>
@@ -22825,15 +23585,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:75" ht="48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>517</v>
+        <v>452</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D2" s="1">
         <v>3</v>
@@ -22845,10 +23605,10 @@
         <v>3</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>403</v>
+        <v>296</v>
       </c>
       <c r="I2" s="35" t="s">
         <v>442</v>
@@ -22863,10 +23623,10 @@
         <v>52</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>44</v>
+        <v>464</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>295</v>
+        <v>524</v>
       </c>
       <c r="O2" s="8" t="s">
         <v>59</v>
@@ -22905,10 +23665,10 @@
         <v>246</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>521</v>
+        <v>537</v>
       </c>
       <c r="AB2" s="12" t="s">
-        <v>520</v>
+        <v>537</v>
       </c>
       <c r="AC2" s="9" t="s">
         <v>69</v>
@@ -22940,8 +23700,8 @@
       <c r="AL2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AM2" s="7">
-        <v>0</v>
+      <c r="AM2" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="AN2" s="13" t="s">
         <v>281</v>
@@ -22956,13 +23716,13 @@
         <v>139</v>
       </c>
       <c r="AR2" s="7" t="s">
-        <v>429</v>
+        <v>139</v>
       </c>
       <c r="AS2" s="13" t="s">
-        <v>292</v>
+        <v>522</v>
       </c>
       <c r="AT2" s="13" t="s">
-        <v>292</v>
+        <v>522</v>
       </c>
       <c r="AU2" s="13" t="s">
         <v>498</v>
@@ -23013,7 +23773,7 @@
         <v>156</v>
       </c>
       <c r="BK2" s="7" t="s">
-        <v>522</v>
+        <v>290</v>
       </c>
       <c r="BL2" s="7">
         <v>123</v>
@@ -23049,113 +23809,1690 @@
         <v>9</v>
       </c>
       <c r="BW2" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="3" spans="1:75" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R3" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="Z3" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA3" s="12" t="s">
+        <v>535</v>
+      </c>
+      <c r="AB3" s="12" t="s">
+        <v>536</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK3" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN3" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO3" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP3" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ3" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR3" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS3" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT3" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU3" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ3" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA3" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB3" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC3" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD3" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE3" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF3" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH3" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK3" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL3" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM3" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BN3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP3" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS3" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT3" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU3" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW3" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:75" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R4" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="Z4" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA4" s="12" t="s">
+        <v>528</v>
+      </c>
+      <c r="AB4" s="12" t="s">
+        <v>529</v>
+      </c>
+      <c r="AC4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK4" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN4" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO4" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ4" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="AR4" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="AS4" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT4" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AV4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ4" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA4" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB4" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC4" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD4" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE4" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF4" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH4" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI4" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK4" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL4" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM4" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BN4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP4" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS4" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT4" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU4" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW4" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:75" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R5" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="Z5" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA5" s="12" t="s">
+        <v>530</v>
+      </c>
+      <c r="AB5" s="12" t="s">
+        <v>531</v>
+      </c>
+      <c r="AC5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE5" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK5" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN5" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO5" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ5" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="AR5" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="AS5" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="AT5" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="AU5" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AV5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ5" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA5" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="BB5" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="BC5" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="BD5" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE5" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF5" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH5" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI5" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK5" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL5" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM5" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BN5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP5" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS5" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT5" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU5" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW5" s="7" t="s">
         <v>443</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="32">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2" xr:uid="{D3900C6F-1777-4D0B-830B-6CA38C678C2E}">
+  <dataValidations count="35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2:AU5" xr:uid="{EC928448-8EC4-4CB1-A994-D1C9228B148B}">
       <formula1>"LCC,LCC+GDS,GDS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{87E15701-8FFF-47C6-8182-91C969B70A45}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5" xr:uid="{0DDC40CB-7A4C-40BF-B31C-4A553525E5FD}">
       <formula1>"Normal,SSO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{33668CE0-1DDE-45B3-82C9-A3877A20A5C6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H5" xr:uid="{CAD0730E-A63B-4E21-B91B-FED4529C8D74}">
       <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{923274EF-88F2-49F5-95F7-51E925A08275}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M5" xr:uid="{A2363397-B5A7-47AC-B91F-37630D3394E0}">
       <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2 BW2" xr:uid="{4BDDF4B7-CD7E-4D4D-BD02-4E9D70AECE6F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K5 BW2:BW5" xr:uid="{AC4E50D1-7B4E-45C1-B0F9-BE54B4057BCA}">
       <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur,D Divaker S,Ankur Yadav,Sachin Kumar"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2" xr:uid="{277A127C-28B8-4779-9E1B-8EA1452D0880}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z5" xr:uid="{4E2059D6-DF67-4F2E-A9F8-955F0911D857}">
       <formula1>"Business trip  - Without reason"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AR2" xr:uid="{E7EC7AA6-D0C3-449C-904C-FB0B98DC357A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AR3" xr:uid="{5A7ECA39-CA67-4022-986F-8D2A58856DE9}">
       <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{E23F84D7-0B2D-4F2B-B8C8-4359E60D88E7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P5" xr:uid="{309F1BC4-FAA4-447C-B9E4-DAB83AD1DFD8}">
       <formula1>"On,Off"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP2 AK2 AN2 BS2" xr:uid="{B35E8AC8-02E1-4306-BCD3-04FB4439816E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP2:AP5 AK2:AK5 AN2:AN5 BS2:BS5" xr:uid="{1216AF12-4212-4634-895A-AD628A51B2C3}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2" xr:uid="{BD05D512-9370-49E0-A144-2FCFC60ECE24}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2:BR5" xr:uid="{0135A625-9D4A-425E-9572-EE947EAC85DA}">
       <formula1>"Hold and quote,Quote,Fullfillment"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BM2" xr:uid="{56300E86-4641-4666-8550-5E9D4BFDDFC1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BM2:BM5" xr:uid="{B2219BA7-5CA3-453D-B13D-DC33DDD92D73}">
       <formula1>"Trip Request,Flight Book,Addtocart"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{DE2D710D-048B-4747-9987-1BD7E2250EA3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L5" xr:uid="{54D4D5EE-8109-4DBE-B4D5-EC79E251D682}">
       <formula1>"Administrator,Travel Arranger,Employee"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{495278D9-DCC7-4117-BC8F-9DDA1A0D934D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5" xr:uid="{DD205B55-E6B4-4B43-A0CF-B8932BCE1533}">
       <formula1>"sbt,preprod117"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2 BO2 C2" xr:uid="{37380F4F-37F7-4632-BE33-5BBDCC35E971}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2:AC5 BO2:BO5 C2:C5" xr:uid="{490C6FE3-836B-421F-916C-94E059B880CE}">
       <formula1>"Applied,NotApplied"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{CCE50C8E-E3E4-4C0E-B718-31874734F583}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O5" xr:uid="{ACF4D5A4-0DC7-43D7-AC38-4DD5CCD07329}">
       <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AH2" xr:uid="{69A8293C-E3E1-4D27-89B7-D543D13FEB28}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AH5" xr:uid="{118BEC9A-4E65-412C-8629-C748C84A86B0}">
       <formula1>"0,1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{B2DF9EA9-6765-4431-9EC4-D1DCE05F9A50}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2:AM5" xr:uid="{3ACACE3E-B225-4F0A-B26D-CBF744565CFD}">
       <formula1>"0,1,2,Null"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2" xr:uid="{0E8A5A80-3075-4DAB-8D97-7F82CD8EACE5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2:BK5" xr:uid="{5482CDEC-BB45-4E6F-B005-CE780F5E693D}">
       <formula1>"Master Card,Visa"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2" xr:uid="{504C6EAE-0F0A-446C-A27B-71C58E3AD7CF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S5" xr:uid="{F11BE9FA-A48A-42A4-9D91-371A1BBB943C}">
       <formula1>"Individual,Guest,Personal,Dependent"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2" xr:uid="{13BFBF4F-8F42-4489-9200-DB8F77D7D716}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T5" xr:uid="{B9446D96-4D8B-4F57-91A4-E907AD141DC4}">
       <formula1>"Domestic,International"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2" xr:uid="{7B17BA7E-3C8E-4387-B1CE-E1DB7ADD75D7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U5" xr:uid="{72E96D30-2C65-40E9-82F2-CB8E50751A53}">
       <formula1>"OneWay,RoundTrip"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2" xr:uid="{259CCC1A-E85C-4116-82A5-26588349065F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2:AY5" xr:uid="{CB30D557-953E-4C20-BBF5-4DE6D7BDCCCF}">
       <formula1>"Flight,Flight+Hotel,Flight+Car,Flight+Hotel+Car,Flight+Car+Hotel"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2 D2" xr:uid="{6FD257E7-09EA-47DA-9986-D991407A7B04}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD5 D2:D5" xr:uid="{FB68D6E9-5ECC-441B-BE2A-7D17A66A7959}">
       <formula1>"1,2,3,4,5,6,7,8"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2" xr:uid="{B86F4493-CEC8-4EFD-B94F-39C2984F13F1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL5" xr:uid="{59018923-A5B7-45E4-B7E4-246176AE1F92}">
       <formula1>"InPolicy,OutPolicy,Null"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{3BAA1A34-724C-44CD-AA5B-323690C7704D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q5" xr:uid="{218FCD4E-2907-4A24-B5EF-9AA80BB04E34}">
       <formula1>"Old,New"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2" xr:uid="{63ACD46A-8FFA-4253-BECC-27D42285FD7F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2:BH5" xr:uid="{27BCB8B8-8374-490A-9916-F9ADD6E1CB71}">
       <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2" xr:uid="{155D8940-388F-4386-A78A-97D04D57775F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2:BI5" xr:uid="{B547B30C-AAEA-4DD9-B9DB-33C54B0A300F}">
       <formula1>"1,2,3,4,5,6"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{EF5A522C-150B-410F-89E1-A78425F14AD5}">
-      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AT2" xr:uid="{2EACF76F-2D13-43C3-8D7C-B86423F97D43}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS3:AT4" xr:uid="{5817BC27-B89A-41E7-B56D-145D193549AC}">
       <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare,ECO LITE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2" xr:uid="{C39DAB6B-42EE-4E9B-9997-722A0980A03F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2:AO5" xr:uid="{DEBDD3C3-A254-4C53-BBF4-91BE8405B65C}">
       <formula1>"Duration,Layover,TimingFilter"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{87A79131-0DC0-4B75-A9CF-B7450A8DAF89}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I5" xr:uid="{7EBD3EEA-799E-48E4-8A26-90D932288DC4}">
       <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com,ankit.singh@quadlabs.com"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{6E9686C3-5E56-48D4-83EE-75241BE8EF2B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R5" xr:uid="{AC75DA0E-5022-431F-A98F-549C17D73FC6}">
       <formula1>"prince.chaurasia@quadlabs.com,ayushi.shivhare@quadlabs.com,laxmi.khanal@quadlabs.com,shubham.natkar@quadlabs.com,piyush.chauhan@quadlabs.com,ankur.yadav@quadlabs.com,sachin.kumar@quadlabs.com,ankit.bist@quadlabs.com,ajit.kumar@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS5:AT5" xr:uid="{25A687DB-AFBC-4A4F-8CBC-8F6EB1362E2D}">
+      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare,ECO LITE,ECO VALUE,ECONOMY COMFORT"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AT2" xr:uid="{EB145F55-8FE1-49E3-A98C-7AFA4557B7C2}">
+      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare,ECO LITE,ECO VALUE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N5" xr:uid="{990C8E4F-D679-45B5-80C8-4B4ADAF291A3}">
+      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M,4CJDOMEL9TNCR1R"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ4:AR5" xr:uid="{74D89A81-4565-4484-8ED5-1E3685D76855}">
+      <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet,Oman Air"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" display="Admin@123" xr:uid="{7F0E7733-1EF9-43C3-8A77-5B1C27FAD025}"/>
-    <hyperlink ref="I2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{BB2DB6D9-9D3D-40A8-8CB4-F2B30B699183}"/>
-    <hyperlink ref="R2" r:id="rId3" display="ajit.kumar@quadlabs.com" xr:uid="{55D73720-9660-4207-9DE0-6DF75728F9D4}"/>
+    <hyperlink ref="N2" r:id="rId1" display="Admin@123" xr:uid="{DB86B022-F769-4C7A-9DB9-3FC529F9560F}"/>
+    <hyperlink ref="I2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{5D4920FF-2CED-4A83-AF60-4FE402A0BF11}"/>
+    <hyperlink ref="R2" r:id="rId3" display="ajit.kumar@quadlabs.com" xr:uid="{A60B1C06-5F63-43B7-BFC2-47AE8D93B169}"/>
+    <hyperlink ref="I3:I5" r:id="rId4" display="shekhar.singh@quadlabs.com" xr:uid="{E5F75214-D076-4382-8A97-A8E3BEF0ADBA}"/>
+    <hyperlink ref="N3:N5" r:id="rId5" display="Admin@123" xr:uid="{88796BC8-6CD8-492C-8F80-5F3896C26947}"/>
+    <hyperlink ref="R3:R5" r:id="rId6" display="ajit.kumar@quadlabs.com" xr:uid="{0D8B9D82-0B40-48BF-A17D-EFB642580973}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B6E574-1524-4FC6-990B-395A9F7D764D}">
+  <dimension ref="A1:BW3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="14" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>404</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>406</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA1" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB1" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC1" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK1" s="23" t="s">
+        <v>409</v>
+      </c>
+      <c r="AL1" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="AM1" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="AN1" s="23" t="s">
+        <v>478</v>
+      </c>
+      <c r="AO1" s="23" t="s">
+        <v>477</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="AV1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW1" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AX1" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="AY1" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="AZ1" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="BA1" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="BB1" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="BC1" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="BD1" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="BE1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="BF1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="BG1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="BH1" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="BI1" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="BJ1" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="BK1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="BL1" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="BM1" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="BN1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="BO1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="BS1" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="BT1" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="BU1" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="BV1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="BW1" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:75" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I2" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R2" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="Z2" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA2" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="AB2" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK2" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN2" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO2" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP2" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>522</v>
+      </c>
+      <c r="AT2" s="13" t="s">
+        <v>522</v>
+      </c>
+      <c r="AU2" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AV2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="AZ2" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="BA2" s="13" t="s">
+        <v>539</v>
+      </c>
+      <c r="BB2" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="BC2" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="BD2" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF2" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH2" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK2" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL2" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM2" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BN2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP2" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS2" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT2" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU2" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW2" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="3" spans="1:75" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="R3" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="Z3" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA3" s="12" t="s">
+        <v>536</v>
+      </c>
+      <c r="AB3" s="12" t="s">
+        <v>540</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK3" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN3" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO3" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AP3" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ3" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="AR3" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="AS3" s="13" t="s">
+        <v>522</v>
+      </c>
+      <c r="AT3" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU3" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AV3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AW3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AX3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AY3" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="AZ3" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="BA3" s="13" t="s">
+        <v>541</v>
+      </c>
+      <c r="BB3" s="12" t="s">
+        <v>536</v>
+      </c>
+      <c r="BC3" s="12" t="s">
+        <v>536</v>
+      </c>
+      <c r="BD3" s="7">
+        <v>78554432323</v>
+      </c>
+      <c r="BE3" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF3" s="7">
+        <v>345678</v>
+      </c>
+      <c r="BG3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH3" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK3" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BL3" s="7">
+        <v>123</v>
+      </c>
+      <c r="BM3" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BN3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP3" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS3" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="BT3" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU3" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BV3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW3" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AT2 AS3" xr:uid="{2ED64E23-E70B-45DE-A35E-85E5A30CF3D6}">
+      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare,ECO LITE,ECO VALUE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R3" xr:uid="{82F7442D-09B2-4B89-9810-DC7BD179E262}">
+      <formula1>"prince.chaurasia@quadlabs.com,ayushi.shivhare@quadlabs.com,laxmi.khanal@quadlabs.com,shubham.natkar@quadlabs.com,piyush.chauhan@quadlabs.com,ankur.yadav@quadlabs.com,sachin.kumar@quadlabs.com,ankit.bist@quadlabs.com,ajit.kumar@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I3" xr:uid="{4C870F32-8074-451B-ABD2-6CB213734A3C}">
+      <formula1>"shekhar.singh@quadlabs.com,sachin.kumar@quadlabs.com,Laxmi.khanal@quadlabs.com,ayushi.shivhare@quadlabs.com,Vikrant.prajapati@quadlabs.com,ankit.singh@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2:AO3" xr:uid="{A0AF4344-0C99-4029-990C-41AF6E3B5465}">
+      <formula1>"Duration,Layover,TimingFilter"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2:BI3" xr:uid="{42E453F7-1801-4493-91B2-DDB093D058BC}">
+      <formula1>"1,2,3,4,5,6"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2:BH3" xr:uid="{140F3AAD-0367-4044-A3FD-A47E97E97C5D}">
+      <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q3" xr:uid="{712E3F93-DD6B-4D94-943E-590142101106}">
+      <formula1>"Old,New"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL3" xr:uid="{67072100-EE9D-4DB7-BD4E-C76C740B0F0B}">
+      <formula1>"InPolicy,OutPolicy,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD3 D2:D3" xr:uid="{9A4AD928-0CDA-410B-BC2E-AC371BA98256}">
+      <formula1>"1,2,3,4,5,6,7,8"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2:AY3" xr:uid="{24444412-772A-4700-A19C-667FB9D8CBC0}">
+      <formula1>"Flight,Flight+Hotel,Flight+Car,Flight+Hotel+Car,Flight+Car+Hotel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3" xr:uid="{2AB4B260-5963-4333-B466-880BF67014B7}">
+      <formula1>"OneWay,RoundTrip"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T3" xr:uid="{E07BF0FA-229F-451C-9FAF-7F74E9740E1E}">
+      <formula1>"Domestic,International"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S3" xr:uid="{1D554BA9-10F1-427E-BD41-74792659D624}">
+      <formula1>"Individual,Guest,Personal,Dependent"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2:BK3" xr:uid="{F329C05C-F093-4B60-A969-9E0C9178B39E}">
+      <formula1>"Master Card,Visa"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2:AM3" xr:uid="{76B64032-3675-4BD2-941B-3C8541596F64}">
+      <formula1>"0,1,2,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AH3" xr:uid="{40AAB1AB-2C55-42B6-B72D-5238350289F4}">
+      <formula1>"0,1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3" xr:uid="{879DE0FF-0874-4C80-AFC2-FC51A9DA992B}">
+      <formula1>"Poonam_Corp,Amazon,Demo Corporate,Lux_Test_corp,Null"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2:AC3 BO2:BO3 C2:C3" xr:uid="{76D8315B-7A74-4A8E-8BB6-DDF055ABB714}">
+      <formula1>"Applied,NotApplied"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{0F3465E6-7EA8-41E5-9F7D-DF8BFEA1BA4D}">
+      <formula1>"sbt,preprod117"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L3" xr:uid="{75B9222A-24F4-4FF2-AE27-CE81883117AF}">
+      <formula1>"Administrator,Travel Arranger,Employee"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BM2:BM3" xr:uid="{DE3974ED-D9BB-48BF-952B-C2A06C1C740F}">
+      <formula1>"Trip Request,Flight Book,Addtocart"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2:BR3" xr:uid="{98523617-ACB9-40B9-B99A-59A2ED2514A2}">
+      <formula1>"Hold and quote,Quote,Fullfillment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP2:AP3 AK2:AK3 AN2:AN3 BS2:BS3" xr:uid="{5C5D30D0-7713-4058-8D75-48845FA92A69}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3" xr:uid="{E4763A3B-8294-4C0E-8D8C-BDB7090AC714}">
+      <formula1>"On,Off"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AR2" xr:uid="{6419269E-F65B-45E4-9F84-C07FBF389413}">
+      <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z3" xr:uid="{16388B76-E72C-49CB-933D-1ABC0B401BD1}">
+      <formula1>"Business trip  - Without reason"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K3 BW2:BW3" xr:uid="{8E15FDFE-CBA4-4F34-8A9C-8E93C81D8511}">
+      <formula1>"Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur,D Divaker S,Ankur Yadav,Sachin Kumar"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M3" xr:uid="{163C42BE-D264-413D-865A-978A13706B53}">
+      <formula1>"Shubham1,Shubham,rsudesh15,Saurabh,Laxmi,sachinkumar,Piyush,Ankur"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H3" xr:uid="{AAF84EA6-2908-45E9-8611-87DBFE8938F9}">
+      <formula1>"//staging117/sbt,//preprod.quadlabs.net/sbt/#,test.quadlabs.net/sbt,tripsource.co.in/sbt/#,//test.quadlabs.net/SSO_Login"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3" xr:uid="{BC71A964-3271-4927-9F8E-17273260A612}">
+      <formula1>"Normal,SSO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2:AU3" xr:uid="{CA2EB351-ED08-4467-9DC9-D28AAC33ADC2}">
+      <formula1>"LCC,LCC+GDS,GDS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3" xr:uid="{CC244F04-819F-4850-A567-A70EB412443F}">
+      <formula1>"Laxmi@123,Admin@123,S21FUMK6JAPLBYO,Shubham@123,BAVYBXVY09FKGTY,Piyush@123,Ankur@123,DWUFR8WRAR6SL1M,4CJDOMEL9TNCR1R"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AT3" xr:uid="{5EB677E9-C73B-481C-9A3E-6339FF3AA51A}">
+      <formula1>"Economy Saver,Economy Basic,SAVER,Spice Saver,PUB,Flexi Fare,Economy,ECO STANDARD,Standard,SME FARE,Economy Fare,ECO LITE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ3:AR3" xr:uid="{3F7FB19C-291B-4EF2-A916-196719325BB4}">
+      <formula1>"Air India,Vistara,SriLankan,Saudi Arabian,Emirates,Gulf Air,Etihad Airways,Singapore Airl,Qatar Airways,Indigo,Air Asia,Akasa Air,SpiceJet,Oman Air"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" display="Admin@123" xr:uid="{5563FAE7-F7F4-4CB2-8846-184F9E56FB02}"/>
+    <hyperlink ref="I2" r:id="rId2" display="shekhar.singh@quadlabs.com" xr:uid="{6C8D3FD1-0ADA-4164-BC67-D8F6A7692C53}"/>
+    <hyperlink ref="R2" r:id="rId3" display="ajit.kumar@quadlabs.com" xr:uid="{81E72062-10E0-4586-B229-0FAB453BEC89}"/>
+    <hyperlink ref="I3" r:id="rId4" display="shekhar.singh@quadlabs.com" xr:uid="{F5C13127-26CB-4668-89E6-B484ABEFB632}"/>
+    <hyperlink ref="N3" r:id="rId5" display="Admin@123" xr:uid="{4E2F3935-6E3C-422D-B222-F007242E6FD2}"/>
+    <hyperlink ref="R3" r:id="rId6" display="ajit.kumar@quadlabs.com" xr:uid="{6EA1B6B4-8E03-4B2C-8080-D2CA9AC67FEA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>